<commit_message>
Update BCRbQ based on SYC
</commit_message>
<xml_diff>
--- a/InputData/elec/BCRbQ/BAU Cap Retirements before Quantization.xlsx
+++ b/InputData/elec/BCRbQ/BAU Cap Retirements before Quantization.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="14" r:id="rId1"/>
@@ -18,9 +18,6 @@
     <sheet name="SYC-SYEGC" sheetId="20" r:id="rId4"/>
     <sheet name="BCRbQ" sheetId="2" r:id="rId5"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId6"/>
-  </externalReferences>
   <definedNames>
     <definedName name="Countries">#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Gross Capacities'!$1:$1</definedName>
@@ -30,7 +27,7 @@
     <definedName name="qry_units_readout_full">#REF!</definedName>
     <definedName name="qry_units_readout_headline">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcCompleted="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -868,178 +865,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="About"/>
-      <sheetName val="nrg_inf_epc"/>
-      <sheetName val="nrg_inf_epcrw"/>
-      <sheetName val="nrg_inf_epct"/>
-      <sheetName val="Gross Capacities"/>
-      <sheetName val="Thermal Calcs"/>
-      <sheetName val="SYC-SYEGC"/>
-      <sheetName val="SYC-FoPtPFP"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1">
-        <row r="148">
-          <cell r="D148">
-            <v>119214.59</v>
-          </cell>
-        </row>
-        <row r="324">
-          <cell r="D324">
-            <v>104699.452</v>
-          </cell>
-        </row>
-        <row r="412">
-          <cell r="D412">
-            <v>23529.671999999999</v>
-          </cell>
-        </row>
-        <row r="588">
-          <cell r="D588">
-            <v>864.755</v>
-          </cell>
-        </row>
-        <row r="764">
-          <cell r="D764">
-            <v>2306.0129999999999</v>
-          </cell>
-        </row>
-        <row r="852">
-          <cell r="D852">
-            <v>102927.90700000001</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2">
-        <row r="16">
-          <cell r="D16">
-            <v>20584.516</v>
-          </cell>
-        </row>
-        <row r="962">
-          <cell r="D962">
-            <v>11040.941999999999</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5">
-        <row r="13">
-          <cell r="B13">
-            <v>266.75065588015173</v>
-          </cell>
-          <cell r="C13">
-            <v>0</v>
-          </cell>
-          <cell r="D13">
-            <v>2986.4927671734945</v>
-          </cell>
-          <cell r="E13">
-            <v>0</v>
-          </cell>
-          <cell r="F13">
-            <v>89294.796772972259</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14">
-            <v>141975.949524219</v>
-          </cell>
-          <cell r="C14">
-            <v>0</v>
-          </cell>
-          <cell r="D14">
-            <v>11382.431286939533</v>
-          </cell>
-          <cell r="E14">
-            <v>0</v>
-          </cell>
-          <cell r="F14">
-            <v>22184.449830479447</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15">
-            <v>498.99520906037816</v>
-          </cell>
-          <cell r="C15">
-            <v>5301.1367742096845</v>
-          </cell>
-          <cell r="D15">
-            <v>2821.6581960982489</v>
-          </cell>
-          <cell r="E15">
-            <v>0</v>
-          </cell>
-          <cell r="F15">
-            <v>333.21033054744692</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17">
-            <v>0</v>
-          </cell>
-          <cell r="C17">
-            <v>14159.565225790318</v>
-          </cell>
-          <cell r="D17">
-            <v>0</v>
-          </cell>
-          <cell r="E17">
-            <v>0</v>
-          </cell>
-          <cell r="F17">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="B18">
-            <v>0</v>
-          </cell>
-          <cell r="C18">
-            <v>0</v>
-          </cell>
-          <cell r="D18">
-            <v>1542.5277497887241</v>
-          </cell>
-          <cell r="E18">
-            <v>0</v>
-          </cell>
-          <cell r="F18">
-            <v>50739.513373591297</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="B19">
-            <v>1003.7446108404566</v>
-          </cell>
-          <cell r="C19">
-            <v>0</v>
-          </cell>
-          <cell r="D19">
-            <v>0</v>
-          </cell>
-          <cell r="E19">
-            <v>0</v>
-          </cell>
-          <cell r="F19">
-            <v>16735.292692409552</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1305,7 +1130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1482,7 +1307,7 @@
   <dimension ref="A1:AZ209"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
       <selection pane="topRight" activeCell="B2" sqref="B2"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
@@ -40183,8 +40008,8 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -40220,7 +40045,6 @@
         <v>20</v>
       </c>
       <c r="B2" s="1">
-        <f>SUM('[1]Thermal Calcs'!B13:F13)</f>
         <v>92548.040196025904</v>
       </c>
       <c r="C2">
@@ -40243,7 +40067,6 @@
         <v>10</v>
       </c>
       <c r="B3" s="1">
-        <f>SUM('[1]Thermal Calcs'!B14:F14)</f>
         <v>175542.83064163799</v>
       </c>
       <c r="C3">
@@ -40266,7 +40089,6 @@
         <v>0</v>
       </c>
       <c r="B4" s="1">
-        <f>[1]nrg_inf_epc!D148</f>
         <v>119214.59</v>
       </c>
       <c r="C4">
@@ -40289,7 +40111,6 @@
         <v>1</v>
       </c>
       <c r="B5" s="40">
-        <f>[1]nrg_inf_epc!D324+[1]nrg_inf_epc!D412</f>
         <v>128229.12400000001</v>
       </c>
       <c r="C5">
@@ -40334,7 +40155,6 @@
         <v>79</v>
       </c>
       <c r="B7" s="40">
-        <f>[1]nrg_inf_epc!D852</f>
         <v>102927.90700000001</v>
       </c>
       <c r="C7">
@@ -40357,7 +40177,6 @@
         <v>3</v>
       </c>
       <c r="B8" s="40">
-        <f>[1]nrg_inf_epc!D764</f>
         <v>2306.0129999999999</v>
       </c>
       <c r="C8">
@@ -40380,7 +40199,6 @@
         <v>4</v>
       </c>
       <c r="B9" s="40">
-        <f>[1]nrg_inf_epcrw!D16</f>
         <v>20584.516</v>
       </c>
       <c r="C9">
@@ -40403,7 +40221,6 @@
         <v>5</v>
       </c>
       <c r="B10" s="40">
-        <f>[1]nrg_inf_epc!D588</f>
         <v>864.755</v>
       </c>
       <c r="C10">
@@ -40426,7 +40243,6 @@
         <v>11</v>
       </c>
       <c r="B11" s="40">
-        <f>SUM('[1]Thermal Calcs'!B15:F15)</f>
         <v>8955.0005099157588</v>
       </c>
       <c r="C11">
@@ -40449,7 +40265,6 @@
         <v>12</v>
       </c>
       <c r="B12" s="40">
-        <f>SUM('[1]Thermal Calcs'!B17:F17)</f>
         <v>14159.565225790318</v>
       </c>
       <c r="C12">
@@ -40472,7 +40287,6 @@
         <v>18</v>
       </c>
       <c r="B13" s="40">
-        <f>SUM('[1]Thermal Calcs'!B18:F18)</f>
         <v>52282.041123380019</v>
       </c>
       <c r="C13">
@@ -40538,7 +40352,6 @@
         <v>31</v>
       </c>
       <c r="B16" s="1">
-        <f>SUM('[1]Thermal Calcs'!B19:F19)</f>
         <v>17739.03730325001</v>
       </c>
       <c r="C16">
@@ -40561,7 +40374,6 @@
         <v>32</v>
       </c>
       <c r="B17" s="1">
-        <f>[1]nrg_inf_epcrw!D962</f>
         <v>11040.941999999999</v>
       </c>
       <c r="C17">
@@ -40591,7 +40403,9 @@
   </sheetPr>
   <dimension ref="A1:AJ23"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:AH15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -40709,136 +40523,136 @@
         <v>20</v>
       </c>
       <c r="B2" s="1">
-        <f>jrc_potencia!T5</f>
-        <v>2441</v>
+        <f>jrc_potencia!T5*'SYC-SYEGC'!$G$2</f>
+        <v>2195.2184839228812</v>
       </c>
       <c r="C2" s="1">
-        <f>jrc_potencia!U5</f>
-        <v>3440</v>
+        <f>jrc_potencia!U5*'SYC-SYEGC'!$G$2</f>
+        <v>3093.6303091744003</v>
       </c>
       <c r="D2" s="1">
-        <f>jrc_potencia!V5</f>
-        <v>4624.0399999999936</v>
+        <f>jrc_potencia!V5*'SYC-SYEGC'!$G$2</f>
+        <v>4158.4506671031322</v>
       </c>
       <c r="E2" s="1">
-        <f>jrc_potencia!W5</f>
-        <v>4542.3000000000029</v>
+        <f>jrc_potencia!W5*'SYC-SYEGC'!$G$2</f>
+        <v>4084.9409748147928</v>
       </c>
       <c r="F2" s="1">
-        <f>jrc_potencia!X5</f>
-        <v>5332.4079999999958</v>
+        <f>jrc_potencia!X5*'SYC-SYEGC'!$G$2</f>
+        <v>4795.4938981639625</v>
       </c>
       <c r="G2" s="1">
-        <f>jrc_potencia!Y5</f>
-        <v>2102.2000000000116</v>
+        <f>jrc_potencia!Y5*'SYC-SYEGC'!$G$2</f>
+        <v>1890.5318709146686</v>
       </c>
       <c r="H2" s="1">
-        <f>jrc_potencia!Z5</f>
-        <v>6015.4510000000009</v>
+        <f>jrc_potencia!Z5*'SYC-SYEGC'!$G$2</f>
+        <v>5409.7620746957728</v>
       </c>
       <c r="I2" s="1">
-        <f>jrc_potencia!AA5</f>
-        <v>1972.7999999999884</v>
+        <f>jrc_potencia!AA5*'SYC-SYEGC'!$G$2</f>
+        <v>1774.1610098660526</v>
       </c>
       <c r="J2" s="1">
-        <f>jrc_potencia!AB5</f>
-        <v>1927.4000000000087</v>
+        <f>jrc_potencia!AB5*'SYC-SYEGC'!$G$2</f>
+        <v>1733.3322842740599</v>
       </c>
       <c r="K2" s="1">
-        <f>jrc_potencia!AC5</f>
-        <v>3470.9619999999995</v>
+        <f>jrc_potencia!AC5*'SYC-SYEGC'!$G$2</f>
+        <v>3121.4747805792422</v>
       </c>
       <c r="L2" s="1">
-        <f>jrc_potencia!AD5</f>
-        <v>1027.8999999999942</v>
+        <f>jrc_potencia!AD5*'SYC-SYEGC'!$G$2</f>
+        <v>924.40191709312444</v>
       </c>
       <c r="M2" s="1">
-        <f>jrc_potencia!AE5</f>
-        <v>3733.2000000000044</v>
+        <f>jrc_potencia!AE5*'SYC-SYEGC'!$G$2</f>
+        <v>3357.3083343633384</v>
       </c>
       <c r="N2" s="1">
-        <f>jrc_potencia!AF5</f>
-        <v>5916.6339999999982</v>
+        <f>jrc_potencia!AF5*'SYC-SYEGC'!$G$2</f>
+        <v>5320.8948461313266</v>
       </c>
       <c r="O2" s="1">
-        <f>jrc_potencia!AG5</f>
-        <v>2483</v>
+        <f>jrc_potencia!AG5*'SYC-SYEGC'!$G$2</f>
+        <v>2232.9895516511733</v>
       </c>
       <c r="P2" s="1">
-        <f>jrc_potencia!AH5</f>
-        <v>4200.5999999999985</v>
+        <f>jrc_potencia!AH5*'SYC-SYEGC'!$G$2</f>
+        <v>3777.6463595110408</v>
       </c>
       <c r="Q2" s="1">
-        <f>jrc_potencia!AI5</f>
-        <v>5204.4000000000015</v>
+        <f>jrc_potencia!AI5*'SYC-SYEGC'!$G$2</f>
+        <v>4680.3748782172252</v>
       </c>
       <c r="R2" s="1">
-        <f>jrc_potencia!AJ5</f>
-        <v>2105.9499999999971</v>
+        <f>jrc_potencia!AJ5*'SYC-SYEGC'!$G$2</f>
+        <v>1893.9042876761102</v>
       </c>
       <c r="S2" s="1">
-        <f>jrc_potencia!AK5</f>
-        <v>3673.3000000000029</v>
+        <f>jrc_potencia!AK5*'SYC-SYEGC'!$G$2</f>
+        <v>3303.4395972937018</v>
       </c>
       <c r="T2" s="1">
-        <f>jrc_potencia!AL5</f>
-        <v>2720.1999999999971</v>
+        <f>jrc_potencia!AL5*'SYC-SYEGC'!$G$2</f>
+        <v>2446.3061532023821</v>
       </c>
       <c r="U2" s="1">
-        <f>jrc_potencia!AM5</f>
-        <v>2662.8499999999985</v>
+        <f>jrc_potencia!AM5*'SYC-SYEGC'!$G$2</f>
+        <v>2394.7306595305372</v>
       </c>
       <c r="V2" s="1">
-        <f>jrc_potencia!AN5</f>
-        <v>2789.8000000000029</v>
+        <f>jrc_potencia!AN5*'SYC-SYEGC'!$G$2</f>
+        <v>2508.8982082949856</v>
       </c>
       <c r="W2" s="1">
-        <f>jrc_potencia!AO5</f>
-        <v>2366.0499999999993</v>
+        <f>jrc_potencia!AO5*'SYC-SYEGC'!$G$2</f>
+        <v>2127.8151142506067</v>
       </c>
       <c r="X2" s="1">
-        <f>jrc_potencia!AP5</f>
-        <v>1937.4999999999964</v>
+        <f>jrc_potencia!AP5*'SYC-SYEGC'!$G$2</f>
+        <v>1742.4153267515667</v>
       </c>
       <c r="Y2" s="1">
-        <f>jrc_potencia!AQ5</f>
-        <v>1085.7000000000007</v>
+        <f>jrc_potencia!AQ5*'SYC-SYEGC'!$G$2</f>
+        <v>976.38210077635131</v>
       </c>
       <c r="Z2" s="1">
-        <f>jrc_potencia!AR5</f>
-        <v>1512.9000000000015</v>
+        <f>jrc_potencia!AR5*'SYC-SYEGC'!$G$2</f>
+        <v>1360.567818241266</v>
       </c>
       <c r="AA2" s="1">
-        <f>jrc_potencia!AS5</f>
-        <v>450.39999999999782</v>
+        <f>jrc_potencia!AS5*'SYC-SYEGC'!$G$2</f>
+        <v>405.0497358291114</v>
       </c>
       <c r="AB2" s="1">
-        <f>jrc_potencia!AT5</f>
-        <v>430.49999999999636</v>
+        <f>jrc_potencia!AT5*'SYC-SYEGC'!$G$2</f>
+        <v>387.15344421499071</v>
       </c>
       <c r="AC2" s="1">
-        <f>jrc_potencia!AU5</f>
-        <v>653.69999999999709</v>
+        <f>jrc_potencia!AU5*'SYC-SYEGC'!$G$2</f>
+        <v>587.87968985677219</v>
       </c>
       <c r="AD2" s="1">
-        <f>jrc_potencia!AV5</f>
-        <v>741.90000000000146</v>
+        <f>jrc_potencia!AV5*'SYC-SYEGC'!$G$2</f>
+        <v>667.19893208618953</v>
       </c>
       <c r="AE2" s="1">
-        <f>jrc_potencia!AW5</f>
-        <v>372</v>
+        <f>jrc_potencia!AW5*'SYC-SYEGC'!$G$2</f>
+        <v>334.5437427363014</v>
       </c>
       <c r="AF2" s="1">
-        <f>jrc_potencia!AX5</f>
-        <v>2935.8000000000029</v>
+        <f>jrc_potencia!AX5*'SYC-SYEGC'!$G$2</f>
+        <v>2640.19763420762</v>
       </c>
       <c r="AG2" s="1">
-        <f>jrc_potencia!AY5</f>
-        <v>617.25</v>
+        <f>jrc_potencia!AY5*'SYC-SYEGC'!$G$2</f>
+        <v>555.09979893543562</v>
       </c>
       <c r="AH2" s="1">
-        <f>jrc_potencia!AZ5</f>
-        <v>47.19999999999709</v>
+        <f>jrc_potencia!AZ5*'SYC-SYEGC'!$G$2</f>
+        <v>42.447485637506595</v>
       </c>
       <c r="AJ2" s="1"/>
     </row>
@@ -40847,136 +40661,136 @@
         <v>10</v>
       </c>
       <c r="B3" s="1">
-        <f>jrc_potencia!T46</f>
-        <v>1403.9736999999968</v>
+        <f>jrc_potencia!T46*'SYC-SYEGC'!$G$3</f>
+        <v>1120.6261784217413</v>
       </c>
       <c r="C3" s="1">
-        <f>jrc_potencia!U46</f>
-        <v>2568.5869999999895</v>
+        <f>jrc_potencia!U46*'SYC-SYEGC'!$G$3</f>
+        <v>2050.1992549816</v>
       </c>
       <c r="D3" s="1">
-        <f>jrc_potencia!V46</f>
-        <v>4184.9938999999977</v>
+        <f>jrc_potencia!V46*'SYC-SYEGC'!$G$3</f>
+        <v>3340.3857357693432</v>
       </c>
       <c r="E3" s="1">
-        <f>jrc_potencia!W46</f>
-        <v>3475.9236000000183</v>
+        <f>jrc_potencia!W46*'SYC-SYEGC'!$G$3</f>
+        <v>2774.4187660737311</v>
       </c>
       <c r="F3" s="1">
-        <f>jrc_potencia!X46</f>
-        <v>3884.9395999999797</v>
+        <f>jrc_potencia!X46*'SYC-SYEGC'!$G$3</f>
+        <v>3100.8878708677203</v>
       </c>
       <c r="G3" s="1">
-        <f>jrc_potencia!Y46</f>
-        <v>5143.4317000000019</v>
+        <f>jrc_potencia!Y46*'SYC-SYEGC'!$G$3</f>
+        <v>4105.3932918716755</v>
       </c>
       <c r="H3" s="1">
-        <f>jrc_potencia!Z46</f>
-        <v>3883.1939199999888</v>
+        <f>jrc_potencia!Z46*'SYC-SYEGC'!$G$3</f>
+        <v>3099.494500958343</v>
       </c>
       <c r="I3" s="1">
-        <f>jrc_potencia!AA46</f>
-        <v>3885.9644500000231</v>
+        <f>jrc_potencia!AA46*'SYC-SYEGC'!$G$3</f>
+        <v>3101.7058874295722</v>
       </c>
       <c r="J3" s="1">
-        <f>jrc_potencia!AB46</f>
-        <v>1685.5607899999854</v>
+        <f>jrc_potencia!AB46*'SYC-SYEGC'!$G$3</f>
+        <v>1345.3838534120828</v>
       </c>
       <c r="K3" s="1">
-        <f>jrc_potencia!AC46</f>
-        <v>3202.1637500000102</v>
+        <f>jrc_potencia!AC46*'SYC-SYEGC'!$G$3</f>
+        <v>2555.9086511685737</v>
       </c>
       <c r="L3" s="1">
-        <f>jrc_potencia!AD46</f>
-        <v>4685.9572600000211</v>
+        <f>jrc_potencia!AD46*'SYC-SYEGC'!$G$3</f>
+        <v>3740.2455448570367</v>
       </c>
       <c r="M3" s="1">
-        <f>jrc_potencia!AE46</f>
-        <v>3282.2276300000076</v>
+        <f>jrc_potencia!AE46*'SYC-SYEGC'!$G$3</f>
+        <v>2619.8141786538922</v>
       </c>
       <c r="N3" s="1">
-        <f>jrc_potencia!AF46</f>
-        <v>3413.3155199999778</v>
+        <f>jrc_potencia!AF46*'SYC-SYEGC'!$G$3</f>
+        <v>2724.4461395004782</v>
       </c>
       <c r="O3" s="1">
-        <f>jrc_potencia!AG46</f>
-        <v>6601.130899999991</v>
+        <f>jrc_potencia!AG46*'SYC-SYEGC'!$G$3</f>
+        <v>5268.902183658196</v>
       </c>
       <c r="P3" s="1">
-        <f>jrc_potencia!AH46</f>
-        <v>9187.9635000000271</v>
+        <f>jrc_potencia!AH46*'SYC-SYEGC'!$G$3</f>
+        <v>7333.6647434944834</v>
       </c>
       <c r="Q3" s="1">
-        <f>jrc_potencia!AI46</f>
-        <v>5655.7079999999833</v>
+        <f>jrc_potencia!AI46*'SYC-SYEGC'!$G$3</f>
+        <v>4514.282883154624</v>
       </c>
       <c r="R3" s="1">
-        <f>jrc_potencia!AJ46</f>
-        <v>6029.1334999999963</v>
+        <f>jrc_potencia!AJ46*'SYC-SYEGC'!$G$3</f>
+        <v>4812.3443005374738</v>
       </c>
       <c r="S3" s="1">
-        <f>jrc_potencia!AK46</f>
-        <v>8061.2460000000137</v>
+        <f>jrc_potencia!AK46*'SYC-SYEGC'!$G$3</f>
+        <v>6434.339402723559</v>
       </c>
       <c r="T3" s="1">
-        <f>jrc_potencia!AL46</f>
-        <v>8012.5580000000027</v>
+        <f>jrc_potencia!AL46*'SYC-SYEGC'!$G$3</f>
+        <v>6395.4775299014327</v>
       </c>
       <c r="U3" s="1">
-        <f>jrc_potencia!AM46</f>
-        <v>7794.0140000000174</v>
+        <f>jrc_potencia!AM46*'SYC-SYEGC'!$G$3</f>
+        <v>6221.0396985253992</v>
       </c>
       <c r="V3" s="1">
-        <f>jrc_potencia!AN46</f>
-        <v>7834.7500000000064</v>
+        <f>jrc_potencia!AN46*'SYC-SYEGC'!$G$3</f>
+        <v>6253.5544301077471</v>
       </c>
       <c r="W3" s="1">
-        <f>jrc_potencia!AO46</f>
-        <v>13740.234999999988</v>
+        <f>jrc_potencia!AO46*'SYC-SYEGC'!$G$3</f>
+        <v>10967.20475509383</v>
       </c>
       <c r="X3" s="1">
-        <f>jrc_potencia!AP46</f>
-        <v>13670.410000000036</v>
+        <f>jrc_potencia!AP46*'SYC-SYEGC'!$G$3</f>
+        <v>10911.471714718326</v>
       </c>
       <c r="Y3" s="1">
-        <f>jrc_potencia!AQ46</f>
-        <v>10715.124999999993</v>
+        <f>jrc_potencia!AQ46*'SYC-SYEGC'!$G$3</f>
+        <v>8552.617175137455</v>
       </c>
       <c r="Z3" s="1">
-        <f>jrc_potencia!AR46</f>
-        <v>6883.8159999999643</v>
+        <f>jrc_potencia!AR46*'SYC-SYEGC'!$G$3</f>
+        <v>5494.5362701868389</v>
       </c>
       <c r="AA3" s="1">
-        <f>jrc_potencia!AS46</f>
-        <v>3891.6661700000177</v>
+        <f>jrc_potencia!AS46*'SYC-SYEGC'!$G$3</f>
+        <v>3106.2568962511937</v>
       </c>
       <c r="AB3" s="1">
-        <f>jrc_potencia!AT46</f>
-        <v>7150.5249999999933</v>
+        <f>jrc_potencia!AT46*'SYC-SYEGC'!$G$3</f>
+        <v>5707.4185253321575</v>
       </c>
       <c r="AC3" s="1">
-        <f>jrc_potencia!AU46</f>
-        <v>15622.768750000025</v>
+        <f>jrc_potencia!AU46*'SYC-SYEGC'!$G$3</f>
+        <v>12469.808829523781</v>
       </c>
       <c r="AD3" s="1">
-        <f>jrc_potencia!AV46</f>
-        <v>9133.9749999999822</v>
+        <f>jrc_potencia!AV46*'SYC-SYEGC'!$G$3</f>
+        <v>7290.5721083306107</v>
       </c>
       <c r="AE3" s="1">
-        <f>jrc_potencia!AW46</f>
-        <v>8005</v>
+        <f>jrc_potencia!AW46*'SYC-SYEGC'!$G$3</f>
+        <v>6389.4448722693742</v>
       </c>
       <c r="AF3" s="1">
-        <f>jrc_potencia!AX46</f>
-        <v>6454.0359999999982</v>
+        <f>jrc_potencia!AX46*'SYC-SYEGC'!$G$3</f>
+        <v>5151.4937196304718</v>
       </c>
       <c r="AG3" s="1">
-        <f>jrc_potencia!AY46</f>
-        <v>5254.8200000000234</v>
+        <f>jrc_potencia!AY46*'SYC-SYEGC'!$G$3</f>
+        <v>4194.3013995875954</v>
       </c>
       <c r="AH3" s="1">
-        <f>jrc_potencia!AZ46</f>
-        <v>3729.1700030051188</v>
+        <f>jrc_potencia!AZ46*'SYC-SYEGC'!$G$3</f>
+        <v>2976.5554220514455</v>
       </c>
       <c r="AJ3" s="1"/>
     </row>
@@ -40985,136 +40799,136 @@
         <v>0</v>
       </c>
       <c r="B4" s="1">
-        <f>jrc_potencia!T3</f>
-        <v>1284</v>
+        <f>jrc_potencia!T3*'SYC-SYEGC'!$G$4</f>
+        <v>1231.5488409029306</v>
       </c>
       <c r="C4" s="1">
-        <f>jrc_potencia!U3</f>
-        <v>2611</v>
+        <f>jrc_potencia!U3*'SYC-SYEGC'!$G$4</f>
+        <v>2504.3411398734825</v>
       </c>
       <c r="D4" s="1">
-        <f>jrc_potencia!V3</f>
-        <v>882</v>
+        <f>jrc_potencia!V3*'SYC-SYEGC'!$G$4</f>
+        <v>845.97046548005039</v>
       </c>
       <c r="E4" s="1">
-        <f>jrc_potencia!W3</f>
+        <f>jrc_potencia!W3*'SYC-SYEGC'!$G$4</f>
         <v>0</v>
       </c>
       <c r="F4" s="1">
-        <f>jrc_potencia!X3</f>
-        <v>4058</v>
+        <f>jrc_potencia!X3*'SYC-SYEGC'!$G$4</f>
+        <v>3892.2314613583271</v>
       </c>
       <c r="G4" s="1">
-        <f>jrc_potencia!Y3</f>
-        <v>7464</v>
+        <f>jrc_potencia!Y3*'SYC-SYEGC'!$G$4</f>
+        <v>7159.0970003889979</v>
       </c>
       <c r="H4" s="1">
-        <f>jrc_potencia!Z3</f>
-        <v>3287</v>
+        <f>jrc_potencia!Z3*'SYC-SYEGC'!$G$4</f>
+        <v>3152.7266667039971</v>
       </c>
       <c r="I4" s="1">
-        <f>jrc_potencia!AA3</f>
-        <v>418</v>
+        <f>jrc_potencia!AA3*'SYC-SYEGC'!$G$4</f>
+        <v>400.92477842478581</v>
       </c>
       <c r="J4" s="1">
-        <f>jrc_potencia!AB3</f>
-        <v>3496</v>
+        <f>jrc_potencia!AB3*'SYC-SYEGC'!$G$4</f>
+        <v>3353.1890559163903</v>
       </c>
       <c r="K4" s="1">
-        <f>jrc_potencia!AC3</f>
+        <f>jrc_potencia!AC3*'SYC-SYEGC'!$G$4</f>
         <v>0</v>
       </c>
       <c r="L4" s="1">
-        <f>jrc_potencia!AD3</f>
-        <v>1614</v>
+        <f>jrc_potencia!AD3*'SYC-SYEGC'!$G$4</f>
+        <v>1548.068402817235</v>
       </c>
       <c r="M4" s="1">
-        <f>jrc_potencia!AE3</f>
-        <v>2700</v>
+        <f>jrc_potencia!AE3*'SYC-SYEGC'!$G$4</f>
+        <v>2589.7055065715826</v>
       </c>
       <c r="N4" s="1">
-        <f>jrc_potencia!AF3</f>
-        <v>9298</v>
+        <f>jrc_potencia!AF3*'SYC-SYEGC'!$G$4</f>
+        <v>8918.1784444824352</v>
       </c>
       <c r="O4" s="1">
-        <f>jrc_potencia!AG3</f>
-        <v>6340</v>
+        <f>jrc_potencia!AG3*'SYC-SYEGC'!$G$4</f>
+        <v>6081.0121895051243</v>
       </c>
       <c r="P4" s="1">
-        <f>jrc_potencia!AH3</f>
-        <v>499.75</v>
+        <f>jrc_potencia!AH3*'SYC-SYEGC'!$G$4</f>
+        <v>479.33530626264758</v>
       </c>
       <c r="Q4" s="1">
-        <f>jrc_potencia!AI3</f>
-        <v>5045</v>
+        <f>jrc_potencia!AI3*'SYC-SYEGC'!$G$4</f>
+        <v>4838.9126965383839</v>
       </c>
       <c r="R4" s="1">
-        <f>jrc_potencia!AJ3</f>
-        <v>4139.75</v>
+        <f>jrc_potencia!AJ3*'SYC-SYEGC'!$G$4</f>
+        <v>3970.6419891961891</v>
       </c>
       <c r="S4" s="1">
-        <f>jrc_potencia!AK3</f>
-        <v>9439</v>
+        <f>jrc_potencia!AK3*'SYC-SYEGC'!$G$4</f>
+        <v>9053.418620936729</v>
       </c>
       <c r="T4" s="1">
-        <f>jrc_potencia!AL3</f>
-        <v>6862.75</v>
+        <f>jrc_potencia!AL3*'SYC-SYEGC'!$G$4</f>
+        <v>6582.4079500830112</v>
       </c>
       <c r="U4" s="1">
-        <f>jrc_potencia!AM3</f>
-        <v>5911.75</v>
+        <f>jrc_potencia!AM3*'SYC-SYEGC'!$G$4</f>
+        <v>5670.2561216572421</v>
       </c>
       <c r="V4" s="1">
-        <f>jrc_potencia!AN3</f>
-        <v>6585</v>
+        <f>jrc_potencia!AN3*'SYC-SYEGC'!$G$4</f>
+        <v>6316.0039854718052</v>
       </c>
       <c r="W4" s="1">
-        <f>jrc_potencia!AO3</f>
-        <v>2620</v>
+        <f>jrc_potencia!AO3*'SYC-SYEGC'!$G$4</f>
+        <v>2512.9734915620543</v>
       </c>
       <c r="X4" s="1">
-        <f>jrc_potencia!AP3</f>
-        <v>2314</v>
+        <f>jrc_potencia!AP3*'SYC-SYEGC'!$G$4</f>
+        <v>2219.4735341506084</v>
       </c>
       <c r="Y4" s="1">
-        <f>jrc_potencia!AQ3</f>
-        <v>4794.9999999999927</v>
+        <f>jrc_potencia!AQ3*'SYC-SYEGC'!$G$4</f>
+        <v>4599.1251496335999</v>
       </c>
       <c r="Z4" s="1">
-        <f>jrc_potencia!AR3</f>
-        <v>2630</v>
+        <f>jrc_potencia!AR3*'SYC-SYEGC'!$G$4</f>
+        <v>2522.5649934382454</v>
       </c>
       <c r="AA4" s="1">
-        <f>jrc_potencia!AS3</f>
-        <v>2637</v>
+        <f>jrc_potencia!AS3*'SYC-SYEGC'!$G$4</f>
+        <v>2529.279044751579</v>
       </c>
       <c r="AB4" s="1">
-        <f>jrc_potencia!AT3</f>
-        <v>1782</v>
+        <f>jrc_potencia!AT3*'SYC-SYEGC'!$G$4</f>
+        <v>1709.2056343372446</v>
       </c>
       <c r="AC4" s="1">
-        <f>jrc_potencia!AU3</f>
-        <v>1659</v>
+        <f>jrc_potencia!AU3*'SYC-SYEGC'!$G$4</f>
+        <v>1591.2301612600947</v>
       </c>
       <c r="AD4" s="1">
-        <f>jrc_potencia!AV3</f>
-        <v>2207</v>
+        <f>jrc_potencia!AV3*'SYC-SYEGC'!$G$4</f>
+        <v>2116.8444640753642</v>
       </c>
       <c r="AE4" s="1">
-        <f>jrc_potencia!AW3</f>
-        <v>1970.1999999999971</v>
+        <f>jrc_potencia!AW3*'SYC-SYEGC'!$G$4</f>
+        <v>1889.7176996471574</v>
       </c>
       <c r="AF4" s="1">
-        <f>jrc_potencia!AX3</f>
-        <v>2997.2000000000044</v>
+        <f>jrc_potencia!AX3*'SYC-SYEGC'!$G$4</f>
+        <v>2874.7649423319849</v>
       </c>
       <c r="AG4" s="1">
-        <f>jrc_potencia!AY3</f>
-        <v>5016.0999999999985</v>
+        <f>jrc_potencia!AY3*'SYC-SYEGC'!$G$4</f>
+        <v>4811.1932561161902</v>
       </c>
       <c r="AH4" s="1">
-        <f>jrc_potencia!AZ3</f>
-        <v>1495</v>
+        <f>jrc_potencia!AZ3*'SYC-SYEGC'!$G$4</f>
+        <v>1433.9295304905615</v>
       </c>
       <c r="AJ4" s="1"/>
     </row>
@@ -41261,136 +41075,136 @@
         <v>21</v>
       </c>
       <c r="B6" s="1">
-        <f>jrc_potencia!T15</f>
-        <v>249.54400000002352</v>
+        <f>jrc_potencia!T15*'SYC-SYEGC'!$G$6</f>
+        <v>244.66446359650291</v>
       </c>
       <c r="C6" s="1">
-        <f>jrc_potencia!U15</f>
-        <v>319.84899999998743</v>
+        <f>jrc_potencia!U15*'SYC-SYEGC'!$G$6</f>
+        <v>313.59473286020665</v>
       </c>
       <c r="D6" s="1">
-        <f>jrc_potencia!V15</f>
-        <v>544.58200000002398</v>
+        <f>jrc_potencia!V15*'SYC-SYEGC'!$G$6</f>
+        <v>533.933346080467</v>
       </c>
       <c r="E6" s="1">
-        <f>jrc_potencia!W15</f>
-        <v>791.90499999999884</v>
+        <f>jrc_potencia!W15*'SYC-SYEGC'!$G$6</f>
+        <v>776.42023869285617</v>
       </c>
       <c r="F6" s="1">
-        <f>jrc_potencia!X15</f>
-        <v>1072.8779999999679</v>
+        <f>jrc_potencia!X15*'SYC-SYEGC'!$G$6</f>
+        <v>1051.8991455392886</v>
       </c>
       <c r="G6" s="1">
-        <f>jrc_potencia!Y15</f>
-        <v>1623.5879999999888</v>
+        <f>jrc_potencia!Y15*'SYC-SYEGC'!$G$6</f>
+        <v>1591.8406658612462</v>
       </c>
       <c r="H6" s="1">
-        <f>jrc_potencia!Z15</f>
-        <v>2843.8349999999919</v>
+        <f>jrc_potencia!Z15*'SYC-SYEGC'!$G$6</f>
+        <v>2788.227185714316</v>
       </c>
       <c r="I6" s="1">
-        <f>jrc_potencia!AA15</f>
-        <v>3933.5153500000015</v>
+        <f>jrc_potencia!AA15*'SYC-SYEGC'!$G$6</f>
+        <v>3856.6001312645067</v>
       </c>
       <c r="J6" s="1">
-        <f>jrc_potencia!AB15</f>
-        <v>4546.315419999999</v>
+        <f>jrc_potencia!AB15*'SYC-SYEGC'!$G$6</f>
+        <v>4457.4176240450779</v>
       </c>
       <c r="K6" s="1">
-        <f>jrc_potencia!AC15</f>
-        <v>6091.5851899999543</v>
+        <f>jrc_potencia!AC15*'SYC-SYEGC'!$G$6</f>
+        <v>5972.4714798336154</v>
       </c>
       <c r="L6" s="1">
-        <f>jrc_potencia!AD15</f>
-        <v>4562.8025600000401</v>
+        <f>jrc_potencia!AD15*'SYC-SYEGC'!$G$6</f>
+        <v>4473.5823776129855</v>
       </c>
       <c r="M6" s="1">
-        <f>jrc_potencia!AE15</f>
-        <v>6039.1419600000372</v>
+        <f>jrc_potencia!AE15*'SYC-SYEGC'!$G$6</f>
+        <v>5921.0537148815565</v>
       </c>
       <c r="N6" s="1">
-        <f>jrc_potencia!AF15</f>
-        <v>6694.4658700000145</v>
+        <f>jrc_potencia!AF15*'SYC-SYEGC'!$G$6</f>
+        <v>6563.5635444991485</v>
       </c>
       <c r="O6" s="1">
-        <f>jrc_potencia!AG15</f>
-        <v>7049.8119400000141</v>
+        <f>jrc_potencia!AG15*'SYC-SYEGC'!$G$6</f>
+        <v>6911.9612443343158</v>
       </c>
       <c r="P6" s="1">
-        <f>jrc_potencia!AH15</f>
-        <v>8226.4460100000433</v>
+        <f>jrc_potencia!AH15*'SYC-SYEGC'!$G$6</f>
+        <v>8065.5876332112275</v>
       </c>
       <c r="Q6" s="1">
-        <f>jrc_potencia!AI15</f>
-        <v>7006.886669999978</v>
+        <f>jrc_potencia!AI15*'SYC-SYEGC'!$G$6</f>
+        <v>6869.8753269838971</v>
       </c>
       <c r="R6" s="1">
-        <f>jrc_potencia!AJ15</f>
-        <v>11269.699369999929</v>
+        <f>jrc_potencia!AJ15*'SYC-SYEGC'!$G$6</f>
+        <v>11049.333789851167</v>
       </c>
       <c r="S6" s="1">
-        <f>jrc_potencia!AK15</f>
-        <v>7904.3629499999806</v>
+        <f>jrc_potencia!AK15*'SYC-SYEGC'!$G$6</f>
+        <v>7749.8025247396627</v>
       </c>
       <c r="T6" s="1">
-        <f>jrc_potencia!AL15</f>
-        <v>9121.2563200000441</v>
+        <f>jrc_potencia!AL15*'SYC-SYEGC'!$G$6</f>
+        <v>8942.9009908425469</v>
       </c>
       <c r="U6" s="1">
-        <f>jrc_potencia!AM15</f>
-        <v>10832.129500000039</v>
+        <f>jrc_potencia!AM15*'SYC-SYEGC'!$G$6</f>
+        <v>10620.320078724053</v>
       </c>
       <c r="V6" s="1">
-        <f>jrc_potencia!AN15</f>
-        <v>9103.1670099999756</v>
+        <f>jrc_potencia!AN15*'SYC-SYEGC'!$G$6</f>
+        <v>8925.1653958052102</v>
       </c>
       <c r="W6" s="1">
-        <f>jrc_potencia!AO15</f>
-        <v>10745.20060000004</v>
+        <f>jrc_potencia!AO15*'SYC-SYEGC'!$G$6</f>
+        <v>10535.090970071744</v>
       </c>
       <c r="X6" s="1">
-        <f>jrc_potencia!AP15</f>
-        <v>10319.833310000075</v>
+        <f>jrc_potencia!AP15*'SYC-SYEGC'!$G$6</f>
+        <v>10118.041231992167</v>
       </c>
       <c r="Y6" s="1">
-        <f>jrc_potencia!AQ15</f>
-        <v>12075.287759999919</v>
+        <f>jrc_potencia!AQ15*'SYC-SYEGC'!$G$6</f>
+        <v>11839.169856111625</v>
       </c>
       <c r="Z6" s="1">
-        <f>jrc_potencia!AR15</f>
-        <v>12333.397209999966</v>
+        <f>jrc_potencia!AR15*'SYC-SYEGC'!$G$6</f>
+        <v>12092.232282511153</v>
       </c>
       <c r="AA6" s="1">
-        <f>jrc_potencia!AS15</f>
-        <v>11038.695000000065</v>
+        <f>jrc_potencia!AS15*'SYC-SYEGC'!$G$6</f>
+        <v>10822.846435819576</v>
       </c>
       <c r="AB6" s="1">
-        <f>jrc_potencia!AT15</f>
-        <v>7801.1369999999879</v>
+        <f>jrc_potencia!AT15*'SYC-SYEGC'!$G$6</f>
+        <v>7648.5950355354134</v>
       </c>
       <c r="AC6" s="1">
-        <f>jrc_potencia!AU15</f>
-        <v>13366.16619999992</v>
+        <f>jrc_potencia!AU15*'SYC-SYEGC'!$G$6</f>
+        <v>13104.806702082118</v>
       </c>
       <c r="AD6" s="1">
-        <f>jrc_potencia!AV15</f>
-        <v>3478.5562500000815</v>
+        <f>jrc_potencia!AV15*'SYC-SYEGC'!$G$6</f>
+        <v>3410.5372158675523</v>
       </c>
       <c r="AE6" s="1">
-        <f>jrc_potencia!AW15</f>
-        <v>3344.3333333334303</v>
+        <f>jrc_potencia!AW15*'SYC-SYEGC'!$G$6</f>
+        <v>3278.938868848184</v>
       </c>
       <c r="AF6" s="1">
-        <f>jrc_potencia!AX15</f>
-        <v>4704.8999999999651</v>
+        <f>jrc_potencia!AX15*'SYC-SYEGC'!$G$6</f>
+        <v>4612.9012710186162</v>
       </c>
       <c r="AG6" s="1">
-        <f>jrc_potencia!AY15</f>
-        <v>10125.504166666651</v>
+        <f>jrc_potencia!AY15*'SYC-SYEGC'!$G$6</f>
+        <v>9927.5119641482779</v>
       </c>
       <c r="AH6" s="1">
-        <f>jrc_potencia!AZ15</f>
-        <v>14643.79166666657</v>
+        <f>jrc_potencia!AZ15*'SYC-SYEGC'!$G$6</f>
+        <v>14357.44972086517</v>
       </c>
       <c r="AJ6" s="1"/>
     </row>
@@ -41399,136 +41213,136 @@
         <v>2</v>
       </c>
       <c r="B7" s="1">
-        <f>jrc_potencia!T17</f>
-        <v>4.9999999988358468E-2</v>
+        <f>jrc_potencia!T17*'SYC-SYEGC'!$G$7</f>
+        <v>3.9374781307348936E-2</v>
       </c>
       <c r="C7" s="1">
-        <f>jrc_potencia!U17</f>
-        <v>4.2829999999812571</v>
+        <f>jrc_potencia!U17*'SYC-SYEGC'!$G$7</f>
+        <v>3.3728437675580514</v>
       </c>
       <c r="D7" s="1">
-        <f>jrc_potencia!V17</f>
-        <v>0.16000000003259629</v>
+        <f>jrc_potencia!V17*'SYC-SYEGC'!$G$7</f>
+        <v>0.12599930023852254</v>
       </c>
       <c r="E7" s="1">
-        <f>jrc_potencia!W17</f>
-        <v>0.59999999997671694</v>
+        <f>jrc_potencia!W17*'SYC-SYEGC'!$G$7</f>
+        <v>0.47249737577986384</v>
       </c>
       <c r="F7" s="1">
-        <f>jrc_potencia!X17</f>
-        <v>1.0643999999738298</v>
+        <f>jrc_potencia!X17*'SYC-SYEGC'!$G$7</f>
+        <v>0.83821034464539634</v>
       </c>
       <c r="G7" s="1">
-        <f>jrc_potencia!Y17</f>
-        <v>2.7095000000263099</v>
+        <f>jrc_potencia!Y17*'SYC-SYEGC'!$G$7</f>
+        <v>2.1337193995627532</v>
       </c>
       <c r="H7" s="1">
-        <f>jrc_potencia!Z17</f>
-        <v>4.5380000000004657</v>
+        <f>jrc_potencia!Z17*'SYC-SYEGC'!$G$7</f>
+        <v>3.5736551522874129</v>
       </c>
       <c r="I7" s="1">
-        <f>jrc_potencia!AA17</f>
-        <v>182.08610000001499</v>
+        <f>jrc_potencia!AA17*'SYC-SYEGC'!$G$7</f>
+        <v>143.39200736555924</v>
       </c>
       <c r="J7" s="1">
-        <f>jrc_potencia!AB17</f>
-        <v>575.66499999997905</v>
+        <f>jrc_potencia!AB17*'SYC-SYEGC'!$G$7</f>
+        <v>453.33366973143399</v>
       </c>
       <c r="K7" s="1">
-        <f>jrc_potencia!AC17</f>
-        <v>100.94000000000233</v>
+        <f>jrc_potencia!AC17*'SYC-SYEGC'!$G$7</f>
+        <v>79.489808521785534</v>
       </c>
       <c r="L7" s="1">
-        <f>jrc_potencia!AD17</f>
-        <v>257</v>
+        <f>jrc_potencia!AD17*'SYC-SYEGC'!$G$7</f>
+        <v>202.38637596689529</v>
       </c>
       <c r="M7" s="1">
-        <f>jrc_potencia!AE17</f>
-        <v>709.59400000001187</v>
+        <f>jrc_potencia!AE17*'SYC-SYEGC'!$G$7</f>
+        <v>558.80217147025485</v>
       </c>
       <c r="N7" s="1">
-        <f>jrc_potencia!AF17</f>
-        <v>988.5</v>
+        <f>jrc_potencia!AF17*'SYC-SYEGC'!$G$7</f>
+        <v>778.43942662753307</v>
       </c>
       <c r="O7" s="1">
-        <f>jrc_potencia!AG17</f>
-        <v>983.15117000002647</v>
+        <f>jrc_potencia!AG17*'SYC-SYEGC'!$G$7</f>
+        <v>774.2272463965694</v>
       </c>
       <c r="P7" s="1">
-        <f>jrc_potencia!AH17</f>
-        <v>1974.1611999999732</v>
+        <f>jrc_potencia!AH17*'SYC-SYEGC'!$G$7</f>
+        <v>1554.6433106710185</v>
       </c>
       <c r="Q7" s="1">
-        <f>jrc_potencia!AI17</f>
-        <v>5168.7462000000232</v>
+        <f>jrc_potencia!AI17*'SYC-SYEGC'!$G$7</f>
+        <v>4070.3650261115413</v>
       </c>
       <c r="R7" s="1">
-        <f>jrc_potencia!AJ17</f>
-        <v>6409.0109999999986</v>
+        <f>jrc_potencia!AJ17*'SYC-SYEGC'!$G$7</f>
+        <v>5047.0681316029859</v>
       </c>
       <c r="S7" s="1">
-        <f>jrc_potencia!AK17</f>
-        <v>13139.531139999977</v>
+        <f>jrc_potencia!AK17*'SYC-SYEGC'!$G$7</f>
+        <v>10347.323304781181</v>
       </c>
       <c r="T7" s="1">
-        <f>jrc_potencia!AL17</f>
-        <v>22080.477320000005</v>
+        <f>jrc_potencia!AL17*'SYC-SYEGC'!$G$7</f>
+        <v>17388.279316786091</v>
       </c>
       <c r="U7" s="1">
-        <f>jrc_potencia!AM17</f>
-        <v>18091.241960000014</v>
+        <f>jrc_potencia!AM17*'SYC-SYEGC'!$G$7</f>
+        <v>14246.773918383791</v>
       </c>
       <c r="V7" s="1">
-        <f>jrc_potencia!AN17</f>
-        <v>9510.4690600000904</v>
+        <f>jrc_potencia!AN17*'SYC-SYEGC'!$G$7</f>
+        <v>7489.4527891000134</v>
       </c>
       <c r="W7" s="1">
-        <f>jrc_potencia!AO17</f>
-        <v>6424.1174599999213</v>
+        <f>jrc_potencia!AO17*'SYC-SYEGC'!$G$7</f>
+        <v>5058.9644027822587</v>
       </c>
       <c r="X7" s="1">
-        <f>jrc_potencia!AP17</f>
-        <v>8065.1069900000002</v>
+        <f>jrc_potencia!AP17*'SYC-SYEGC'!$G$7</f>
+        <v>6351.2364805111874</v>
       </c>
       <c r="Y7" s="1">
-        <f>jrc_potencia!AQ17</f>
-        <v>6511.3988430000609</v>
+        <f>jrc_potencia!AQ17*'SYC-SYEGC'!$G$7</f>
+        <v>5127.6981101549309</v>
       </c>
       <c r="Z7" s="1">
-        <f>jrc_potencia!AR17</f>
-        <v>6383.7552299998933</v>
+        <f>jrc_potencia!AR17*'SYC-SYEGC'!$G$7</f>
+        <v>5027.1793231882975</v>
       </c>
       <c r="AA7" s="1">
-        <f>jrc_potencia!AS17</f>
-        <v>8373.4332300000824</v>
+        <f>jrc_potencia!AS17*'SYC-SYEGC'!$G$7</f>
+        <v>6594.0420459941288</v>
       </c>
       <c r="AB7" s="1">
-        <f>jrc_potencia!AT17</f>
-        <v>14765.372229999921</v>
+        <f>jrc_potencia!AT17*'SYC-SYEGC'!$G$7</f>
+        <v>11627.666052264276</v>
       </c>
       <c r="AC7" s="1">
-        <f>jrc_potencia!AU17</f>
-        <v>21831.407230000012</v>
+        <f>jrc_potencia!AU17*'SYC-SYEGC'!$G$7</f>
+        <v>17192.137710261395</v>
       </c>
       <c r="AD7" s="1">
-        <f>jrc_potencia!AV17</f>
-        <v>3033.1285000000498</v>
+        <f>jrc_potencia!AV17*'SYC-SYEGC'!$G$7</f>
+        <v>2388.5754278479194</v>
       </c>
       <c r="AE7" s="1">
-        <f>jrc_potencia!AW17</f>
-        <v>2837.3919999999343</v>
+        <f>jrc_potencia!AW17*'SYC-SYEGC'!$G$7</f>
+        <v>2234.4337901846211</v>
       </c>
       <c r="AF7" s="1">
-        <f>jrc_potencia!AX17</f>
-        <v>5577.8795000000391</v>
+        <f>jrc_potencia!AX17*'SYC-SYEGC'!$G$7</f>
+        <v>4392.5557104476493</v>
       </c>
       <c r="AG7" s="1">
-        <f>jrc_potencia!AY17</f>
-        <v>7054.3690000000061</v>
+        <f>jrc_potencia!AY17*'SYC-SYEGC'!$G$7</f>
+        <v>5555.2847340202816</v>
       </c>
       <c r="AH7" s="1">
-        <f>jrc_potencia!AZ17</f>
-        <v>5687.2625000000116</v>
+        <f>jrc_potencia!AZ17*'SYC-SYEGC'!$G$7</f>
+        <v>4478.6943445425186</v>
       </c>
       <c r="AJ7" s="1"/>
     </row>
@@ -41537,135 +41351,135 @@
         <v>3</v>
       </c>
       <c r="B8" s="1">
-        <f>jrc_potencia!T18</f>
+        <f>jrc_potencia!T18*'SYC-SYEGC'!$G$8</f>
         <v>0</v>
       </c>
       <c r="C8" s="1">
-        <f>jrc_potencia!U18</f>
+        <f>jrc_potencia!U18*'SYC-SYEGC'!$G$8</f>
         <v>0</v>
       </c>
       <c r="D8" s="1">
-        <f>jrc_potencia!V18</f>
+        <f>jrc_potencia!V18*'SYC-SYEGC'!$G$8</f>
         <v>0</v>
       </c>
       <c r="E8" s="1">
-        <f>jrc_potencia!W18</f>
+        <f>jrc_potencia!W18*'SYC-SYEGC'!$G$8</f>
         <v>0</v>
       </c>
       <c r="F8" s="1">
-        <f>jrc_potencia!X18</f>
+        <f>jrc_potencia!X18*'SYC-SYEGC'!$G$8</f>
         <v>0</v>
       </c>
       <c r="G8" s="1">
-        <f>jrc_potencia!Y18</f>
+        <f>jrc_potencia!Y18*'SYC-SYEGC'!$G$8</f>
         <v>0</v>
       </c>
       <c r="H8" s="1">
-        <f>jrc_potencia!Z18</f>
+        <f>jrc_potencia!Z18*'SYC-SYEGC'!$G$8</f>
         <v>0</v>
       </c>
       <c r="I8" s="1">
-        <f>jrc_potencia!AA18</f>
+        <f>jrc_potencia!AA18*'SYC-SYEGC'!$G$8</f>
         <v>0</v>
       </c>
       <c r="J8" s="1">
-        <f>jrc_potencia!AB18</f>
+        <f>jrc_potencia!AB18*'SYC-SYEGC'!$G$8</f>
         <v>0</v>
       </c>
       <c r="K8" s="1">
-        <f>jrc_potencia!AC18</f>
+        <f>jrc_potencia!AC18*'SYC-SYEGC'!$G$8</f>
         <v>0</v>
       </c>
       <c r="L8" s="1">
-        <f>jrc_potencia!AD18</f>
+        <f>jrc_potencia!AD18*'SYC-SYEGC'!$G$8</f>
         <v>0</v>
       </c>
       <c r="M8" s="1">
-        <f>jrc_potencia!AE18</f>
+        <f>jrc_potencia!AE18*'SYC-SYEGC'!$G$8</f>
         <v>0</v>
       </c>
       <c r="N8" s="1">
-        <f>jrc_potencia!AF18</f>
+        <f>jrc_potencia!AF18*'SYC-SYEGC'!$G$8</f>
         <v>0</v>
       </c>
       <c r="O8" s="1">
-        <f>jrc_potencia!AG18</f>
-        <v>11</v>
+        <f>jrc_potencia!AG18*'SYC-SYEGC'!$G$8</f>
+        <v>10.726095395154129</v>
       </c>
       <c r="P8" s="1">
-        <f>jrc_potencia!AH18</f>
+        <f>jrc_potencia!AH18*'SYC-SYEGC'!$G$8</f>
         <v>0</v>
       </c>
       <c r="Q8" s="1">
-        <f>jrc_potencia!AI18</f>
-        <v>49.899999999999636</v>
+        <f>jrc_potencia!AI18*'SYC-SYEGC'!$G$8</f>
+        <v>48.657469110744287</v>
       </c>
       <c r="R8" s="1">
-        <f>jrc_potencia!AJ18</f>
-        <v>222.80000000000018</v>
+        <f>jrc_potencia!AJ18*'SYC-SYEGC'!$G$8</f>
+        <v>217.25218673094017</v>
       </c>
       <c r="S8" s="1">
-        <f>jrc_potencia!AK18</f>
-        <v>449.70000000000027</v>
+        <f>jrc_potencia!AK18*'SYC-SYEGC'!$G$8</f>
+        <v>438.50228174552859</v>
       </c>
       <c r="T8" s="1">
-        <f>jrc_potencia!AL18</f>
-        <v>416.69999999999982</v>
+        <f>jrc_potencia!AL18*'SYC-SYEGC'!$G$8</f>
+        <v>406.32399556006578</v>
       </c>
       <c r="U8" s="1">
-        <f>jrc_potencia!AM18</f>
-        <v>852.5</v>
+        <f>jrc_potencia!AM18*'SYC-SYEGC'!$G$8</f>
+        <v>831.27239312444499</v>
       </c>
       <c r="V8" s="1">
-        <f>jrc_potencia!AN18</f>
-        <v>300</v>
+        <f>jrc_potencia!AN18*'SYC-SYEGC'!$G$8</f>
+        <v>292.52987441329441</v>
       </c>
       <c r="W8" s="1">
-        <f>jrc_potencia!AO18</f>
-        <v>0.3000000000001819</v>
+        <f>jrc_potencia!AO18*'SYC-SYEGC'!$G$8</f>
+        <v>0.29252987441347178</v>
       </c>
       <c r="X8" s="1">
-        <f>jrc_potencia!AP18</f>
-        <v>12</v>
+        <f>jrc_potencia!AP18*'SYC-SYEGC'!$G$8</f>
+        <v>11.701194976531777</v>
       </c>
       <c r="Y8" s="1">
-        <f>jrc_potencia!AQ18</f>
+        <f>jrc_potencia!AQ18*'SYC-SYEGC'!$G$8</f>
         <v>0</v>
       </c>
       <c r="Z8" s="1">
-        <f>jrc_potencia!AR18</f>
-        <v>50</v>
+        <f>jrc_potencia!AR18*'SYC-SYEGC'!$G$8</f>
+        <v>48.754979068882406</v>
       </c>
       <c r="AA8" s="1">
-        <f>jrc_potencia!AS18</f>
+        <f>jrc_potencia!AS18*'SYC-SYEGC'!$G$8</f>
         <v>0</v>
       </c>
       <c r="AB8" s="1">
-        <f>jrc_potencia!AT18</f>
+        <f>jrc_potencia!AT18*'SYC-SYEGC'!$G$8</f>
         <v>0</v>
       </c>
       <c r="AC8" s="1">
-        <f>jrc_potencia!AU18</f>
+        <f>jrc_potencia!AU18*'SYC-SYEGC'!$G$8</f>
         <v>0</v>
       </c>
       <c r="AD8" s="1">
-        <f>jrc_potencia!AV18</f>
+        <f>jrc_potencia!AV18*'SYC-SYEGC'!$G$8</f>
         <v>0</v>
       </c>
       <c r="AE8" s="1">
-        <f>jrc_potencia!AW18</f>
+        <f>jrc_potencia!AW18*'SYC-SYEGC'!$G$8</f>
         <v>0</v>
       </c>
       <c r="AF8" s="1">
-        <f>jrc_potencia!AX18</f>
+        <f>jrc_potencia!AX18*'SYC-SYEGC'!$G$8</f>
         <v>0</v>
       </c>
       <c r="AG8" s="1">
-        <f>jrc_potencia!AY18</f>
+        <f>jrc_potencia!AY18*'SYC-SYEGC'!$G$8</f>
         <v>0</v>
       </c>
       <c r="AH8" s="1">
-        <f>jrc_potencia!AZ18</f>
+        <f>jrc_potencia!AZ18*'SYC-SYEGC'!$G$8</f>
         <v>0</v>
       </c>
       <c r="AJ8" s="1"/>
@@ -41675,136 +41489,136 @@
         <v>4</v>
       </c>
       <c r="B9" s="1">
-        <f>jrc_potencia!T12</f>
-        <v>57.500000000003638</v>
+        <f>jrc_potencia!T12*'SYC-SYEGC'!$G$9</f>
+        <v>50.586211461437379</v>
       </c>
       <c r="C9" s="1">
-        <f>jrc_potencia!U12</f>
-        <v>35</v>
+        <f>jrc_potencia!U12*'SYC-SYEGC'!$G$9</f>
+        <v>30.791606976525152</v>
       </c>
       <c r="D9" s="1">
-        <f>jrc_potencia!V12</f>
-        <v>354.84999999999491</v>
+        <f>jrc_potencia!V12*'SYC-SYEGC'!$G$9</f>
+        <v>312.18290673199408</v>
       </c>
       <c r="E9" s="1">
-        <f>jrc_potencia!W12</f>
-        <v>214.74299999999857</v>
+        <f>jrc_potencia!W12*'SYC-SYEGC'!$G$9</f>
+        <v>188.92234448456847</v>
       </c>
       <c r="F9" s="1">
-        <f>jrc_potencia!X12</f>
-        <v>169.29999999999927</v>
+        <f>jrc_potencia!X12*'SYC-SYEGC'!$G$9</f>
+        <v>148.94340174644816</v>
       </c>
       <c r="G9" s="1">
-        <f>jrc_potencia!Y12</f>
-        <v>49.450000000000728</v>
+        <f>jrc_potencia!Y12*'SYC-SYEGC'!$G$9</f>
+        <v>43.504141856834032</v>
       </c>
       <c r="H9" s="1">
-        <f>jrc_potencia!Z12</f>
-        <v>416.13999999999942</v>
+        <f>jrc_potencia!Z12*'SYC-SYEGC'!$G$9</f>
+        <v>366.10340934889024</v>
       </c>
       <c r="I9" s="1">
-        <f>jrc_potencia!AA12</f>
-        <v>200.96000000000276</v>
+        <f>jrc_potencia!AA12*'SYC-SYEGC'!$G$9</f>
+        <v>176.79660965721655</v>
       </c>
       <c r="J9" s="1">
-        <f>jrc_potencia!AB12</f>
-        <v>566.60499999999956</v>
+        <f>jrc_potencia!AB12*'SYC-SYEGC'!$G$9</f>
+        <v>498.47652774097202</v>
       </c>
       <c r="K9" s="1">
-        <f>jrc_potencia!AC12</f>
-        <v>240.17000000000189</v>
+        <f>jrc_potencia!AC12*'SYC-SYEGC'!$G$9</f>
+        <v>211.29200707291727</v>
       </c>
       <c r="L9" s="1">
-        <f>jrc_potencia!AD12</f>
-        <v>120.75499999999374</v>
+        <f>jrc_potencia!AD12*'SYC-SYEGC'!$G$9</f>
+        <v>106.23544287000291</v>
       </c>
       <c r="M9" s="1">
-        <f>jrc_potencia!AE12</f>
-        <v>254.03400000000329</v>
+        <f>jrc_potencia!AE12*'SYC-SYEGC'!$G$9</f>
+        <v>223.48900247641976</v>
       </c>
       <c r="N9" s="1">
-        <f>jrc_potencia!AF12</f>
-        <v>255.7699999999968</v>
+        <f>jrc_potencia!AF12*'SYC-SYEGC'!$G$9</f>
+        <v>225.0162661824497</v>
       </c>
       <c r="O9" s="1">
-        <f>jrc_potencia!AG12</f>
-        <v>207.1050000000032</v>
+        <f>jrc_potencia!AG12*'SYC-SYEGC'!$G$9</f>
+        <v>182.20273608209544</v>
       </c>
       <c r="P9" s="1">
-        <f>jrc_potencia!AH12</f>
-        <v>265.00000000000364</v>
+        <f>jrc_potencia!AH12*'SYC-SYEGC'!$G$9</f>
+        <v>233.13645282226506</v>
       </c>
       <c r="Q9" s="1">
-        <f>jrc_potencia!AI12</f>
-        <v>307</v>
+        <f>jrc_potencia!AI12*'SYC-SYEGC'!$G$9</f>
+        <v>270.08638119409204</v>
       </c>
       <c r="R9" s="1">
-        <f>jrc_potencia!AJ12</f>
-        <v>774.66000000000349</v>
+        <f>jrc_potencia!AJ12*'SYC-SYEGC'!$G$9</f>
+        <v>681.51503601243087</v>
       </c>
       <c r="S9" s="1">
-        <f>jrc_potencia!AK12</f>
-        <v>804.4217499999977</v>
+        <f>jrc_potencia!AK12*'SYC-SYEGC'!$G$9</f>
+        <v>707.69823912481434</v>
       </c>
       <c r="T9" s="1">
-        <f>jrc_potencia!AL12</f>
-        <v>307.95000000000073</v>
+        <f>jrc_potencia!AL12*'SYC-SYEGC'!$G$9</f>
+        <v>270.92215338345551</v>
       </c>
       <c r="U9" s="1">
-        <f>jrc_potencia!AM12</f>
-        <v>453.6820000000007</v>
+        <f>jrc_potencia!AM12*'SYC-SYEGC'!$G$9</f>
+        <v>399.1313667521116</v>
       </c>
       <c r="V9" s="1">
-        <f>jrc_potencia!AN12</f>
-        <v>521.26000000000204</v>
+        <f>jrc_potencia!AN12*'SYC-SYEGC'!$G$9</f>
+        <v>458.58380150238753</v>
       </c>
       <c r="W9" s="1">
-        <f>jrc_potencia!AO12</f>
-        <v>1244.8199999999997</v>
+        <f>jrc_potencia!AO12*'SYC-SYEGC'!$G$9</f>
+        <v>1095.1430913290867</v>
       </c>
       <c r="X9" s="1">
-        <f>jrc_potencia!AP12</f>
-        <v>440.78299999999581</v>
+        <f>jrc_potencia!AP12*'SYC-SYEGC'!$G$9</f>
+        <v>387.7833399409588</v>
       </c>
       <c r="Y9" s="1">
-        <f>jrc_potencia!AQ12</f>
-        <v>328.58999999999651</v>
+        <f>jrc_potencia!AQ12*'SYC-SYEGC'!$G$9</f>
+        <v>289.08040389760833</v>
       </c>
       <c r="Z9" s="1">
-        <f>jrc_potencia!AR12</f>
-        <v>397.42000000000553</v>
+        <f>jrc_potencia!AR12*'SYC-SYEGC'!$G$9</f>
+        <v>349.6342984174513</v>
       </c>
       <c r="AA9" s="1">
-        <f>jrc_potencia!AS12</f>
-        <v>680.14519999999902</v>
+        <f>jrc_potencia!AS12*'SYC-SYEGC'!$G$9</f>
+        <v>598.36467672485901</v>
       </c>
       <c r="AB9" s="1">
-        <f>jrc_potencia!AT12</f>
-        <v>924.10699999999633</v>
+        <f>jrc_potencia!AT12*'SYC-SYEGC'!$G$9</f>
+        <v>812.99255852158899</v>
       </c>
       <c r="AC9" s="1">
-        <f>jrc_potencia!AU12</f>
-        <v>482.91900000000169</v>
+        <f>jrc_potencia!AU12*'SYC-SYEGC'!$G$9</f>
+        <v>424.85291569990289</v>
       </c>
       <c r="AD9" s="1">
-        <f>jrc_potencia!AV12</f>
-        <v>1033.0794999999998</v>
+        <f>jrc_potencia!AV12*'SYC-SYEGC'!$G$9</f>
+        <v>908.86222684300321</v>
       </c>
       <c r="AE9" s="1">
-        <f>jrc_potencia!AW12</f>
-        <v>610.12725000000501</v>
+        <f>jrc_potencia!AW12*'SYC-SYEGC'!$G$9</f>
+        <v>536.765671076236</v>
       </c>
       <c r="AF9" s="1">
-        <f>jrc_potencia!AX12</f>
-        <v>830.37200000000303</v>
+        <f>jrc_potencia!AX12*'SYC-SYEGC'!$G$9</f>
+        <v>730.52823623746394</v>
       </c>
       <c r="AG9" s="1">
-        <f>jrc_potencia!AY12</f>
-        <v>907.44499999999971</v>
+        <f>jrc_potencia!AY12*'SYC-SYEGC'!$G$9</f>
+        <v>798.33399408036735</v>
       </c>
       <c r="AH9" s="1">
-        <f>jrc_potencia!AZ12</f>
-        <v>739.61500000000524</v>
+        <f>jrc_potencia!AZ12*'SYC-SYEGC'!$G$9</f>
+        <v>650.68383982693751</v>
       </c>
       <c r="AJ9" s="1"/>
     </row>
@@ -41813,136 +41627,136 @@
         <v>5</v>
       </c>
       <c r="B10" s="1">
-        <f>jrc_potencia!T19</f>
-        <v>79.100000000000023</v>
+        <f>jrc_potencia!T19*'SYC-SYEGC'!$G$10</f>
+        <v>82.785831159592149</v>
       </c>
       <c r="C10" s="1">
-        <f>jrc_potencia!U19</f>
-        <v>50.800000000000068</v>
+        <f>jrc_potencia!U19*'SYC-SYEGC'!$G$10</f>
+        <v>53.167133032961893</v>
       </c>
       <c r="D10" s="1">
-        <f>jrc_potencia!V19</f>
-        <v>90.599999999999909</v>
+        <f>jrc_potencia!V19*'SYC-SYEGC'!$G$10</f>
+        <v>94.8216978894948</v>
       </c>
       <c r="E10" s="1">
-        <f>jrc_potencia!W19</f>
-        <v>59.700000000000045</v>
+        <f>jrc_potencia!W19*'SYC-SYEGC'!$G$10</f>
+        <v>62.481847284799663</v>
       </c>
       <c r="F10" s="1">
-        <f>jrc_potencia!X19</f>
-        <v>38.299999999999955</v>
+        <f>jrc_potencia!X19*'SYC-SYEGC'!$G$10</f>
+        <v>40.08466919611093</v>
       </c>
       <c r="G10" s="1">
-        <f>jrc_potencia!Y19</f>
-        <v>71.500000000000057</v>
+        <f>jrc_potencia!Y19*'SYC-SYEGC'!$G$10</f>
+        <v>74.831693146786876</v>
       </c>
       <c r="H10" s="1">
-        <f>jrc_potencia!Z19</f>
-        <v>73.600000000000023</v>
+        <f>jrc_potencia!Z19*'SYC-SYEGC'!$G$10</f>
+        <v>77.029547071377777</v>
       </c>
       <c r="I10" s="1">
-        <f>jrc_potencia!AA19</f>
-        <v>56</v>
+        <f>jrc_potencia!AA19*'SYC-SYEGC'!$G$10</f>
+        <v>58.609437989091766</v>
       </c>
       <c r="J10" s="1">
-        <f>jrc_potencia!AB19</f>
+        <f>jrc_potencia!AB19*'SYC-SYEGC'!$G$10</f>
         <v>0</v>
       </c>
       <c r="K10" s="1">
-        <f>jrc_potencia!AC19</f>
-        <v>96</v>
+        <f>jrc_potencia!AC19*'SYC-SYEGC'!$G$10</f>
+        <v>100.47332226701445</v>
       </c>
       <c r="L10" s="1">
-        <f>jrc_potencia!AD19</f>
-        <v>44.999999999999972</v>
+        <f>jrc_potencia!AD19*'SYC-SYEGC'!$G$10</f>
+        <v>47.096869812663002</v>
       </c>
       <c r="M10" s="1">
-        <f>jrc_potencia!AE19</f>
+        <f>jrc_potencia!AE19*'SYC-SYEGC'!$G$10</f>
         <v>0</v>
       </c>
       <c r="N10" s="1">
-        <f>jrc_potencia!AF19</f>
-        <v>1</v>
+        <f>jrc_potencia!AF19*'SYC-SYEGC'!$G$10</f>
+        <v>1.0465971069480673</v>
       </c>
       <c r="O10" s="1">
-        <f>jrc_potencia!AG19</f>
+        <f>jrc_potencia!AG19*'SYC-SYEGC'!$G$10</f>
         <v>0</v>
       </c>
       <c r="P10" s="1">
-        <f>jrc_potencia!AH19</f>
-        <v>1</v>
+        <f>jrc_potencia!AH19*'SYC-SYEGC'!$G$10</f>
+        <v>1.0465971069480673</v>
       </c>
       <c r="Q10" s="1">
-        <f>jrc_potencia!AI19</f>
+        <f>jrc_potencia!AI19*'SYC-SYEGC'!$G$10</f>
         <v>0</v>
       </c>
       <c r="R10" s="1">
-        <f>jrc_potencia!AJ19</f>
-        <v>29.400000000000006</v>
+        <f>jrc_potencia!AJ19*'SYC-SYEGC'!$G$10</f>
+        <v>30.769954944273184</v>
       </c>
       <c r="S10" s="1">
-        <f>jrc_potencia!AK19</f>
-        <v>54.400000000000006</v>
+        <f>jrc_potencia!AK19*'SYC-SYEGC'!$G$10</f>
+        <v>56.934882617974864</v>
       </c>
       <c r="T10" s="1">
-        <f>jrc_potencia!AL19</f>
-        <v>2</v>
+        <f>jrc_potencia!AL19*'SYC-SYEGC'!$G$10</f>
+        <v>2.0931942138961346</v>
       </c>
       <c r="U10" s="1">
-        <f>jrc_potencia!AM19</f>
-        <v>3</v>
+        <f>jrc_potencia!AM19*'SYC-SYEGC'!$G$10</f>
+        <v>3.1397913208442016</v>
       </c>
       <c r="V10" s="1">
-        <f>jrc_potencia!AN19</f>
+        <f>jrc_potencia!AN19*'SYC-SYEGC'!$G$10</f>
         <v>0</v>
       </c>
       <c r="W10" s="1">
-        <f>jrc_potencia!AO19</f>
-        <v>43</v>
+        <f>jrc_potencia!AO19*'SYC-SYEGC'!$G$10</f>
+        <v>45.003675598766897</v>
       </c>
       <c r="X10" s="1">
-        <f>jrc_potencia!AP19</f>
+        <f>jrc_potencia!AP19*'SYC-SYEGC'!$G$10</f>
         <v>0</v>
       </c>
       <c r="Y10" s="1">
-        <f>jrc_potencia!AQ19</f>
-        <v>11</v>
+        <f>jrc_potencia!AQ19*'SYC-SYEGC'!$G$10</f>
+        <v>11.51256817642874</v>
       </c>
       <c r="Z10" s="1">
-        <f>jrc_potencia!AR19</f>
-        <v>5.5500000000000043</v>
+        <f>jrc_potencia!AR19*'SYC-SYEGC'!$G$10</f>
+        <v>5.8086139435617783</v>
       </c>
       <c r="AA10" s="1">
-        <f>jrc_potencia!AS19</f>
+        <f>jrc_potencia!AS19*'SYC-SYEGC'!$G$10</f>
         <v>0</v>
       </c>
       <c r="AB10" s="1">
-        <f>jrc_potencia!AT19</f>
-        <v>24.199999999999996</v>
+        <f>jrc_potencia!AT19*'SYC-SYEGC'!$G$10</f>
+        <v>25.327649988143225</v>
       </c>
       <c r="AC10" s="1">
-        <f>jrc_potencia!AU19</f>
-        <v>20.000000000000114</v>
+        <f>jrc_potencia!AU19*'SYC-SYEGC'!$G$10</f>
+        <v>20.931942138961464</v>
       </c>
       <c r="AD10" s="1">
-        <f>jrc_potencia!AV19</f>
+        <f>jrc_potencia!AV19*'SYC-SYEGC'!$G$10</f>
         <v>0</v>
       </c>
       <c r="AE10" s="1">
-        <f>jrc_potencia!AW19</f>
-        <v>4.3000000000000025</v>
+        <f>jrc_potencia!AW19*'SYC-SYEGC'!$G$10</f>
+        <v>4.5003675598766923</v>
       </c>
       <c r="AF10" s="1">
-        <f>jrc_potencia!AX19</f>
-        <v>12.35</v>
+        <f>jrc_potencia!AX19*'SYC-SYEGC'!$G$10</f>
+        <v>12.92547427080863</v>
       </c>
       <c r="AG10" s="1">
-        <f>jrc_potencia!AY19</f>
+        <f>jrc_potencia!AY19*'SYC-SYEGC'!$G$10</f>
         <v>0</v>
       </c>
       <c r="AH10" s="1">
-        <f>jrc_potencia!AZ19</f>
-        <v>2</v>
+        <f>jrc_potencia!AZ19*'SYC-SYEGC'!$G$10</f>
+        <v>2.0931942138961346</v>
       </c>
       <c r="AJ10" s="1"/>
     </row>
@@ -41951,135 +41765,135 @@
         <v>11</v>
       </c>
       <c r="B11" s="7">
-        <f>jrc_potencia!T10</f>
-        <v>595.57179999999789</v>
+        <f>jrc_potencia!T10*'SYC-SYEGC'!$G$11</f>
+        <v>611.08992779009372</v>
       </c>
       <c r="C11" s="7">
-        <f>jrc_potencia!U10</f>
-        <v>312.34004000000095</v>
+        <f>jrc_potencia!U10*'SYC-SYEGC'!$G$11</f>
+        <v>320.4783243423484</v>
       </c>
       <c r="D11" s="7">
-        <f>jrc_potencia!V10</f>
-        <v>627.63400000000001</v>
+        <f>jrc_potencia!V10*'SYC-SYEGC'!$G$11</f>
+        <v>643.98753557272028</v>
       </c>
       <c r="E11" s="7">
-        <f>jrc_potencia!W10</f>
-        <v>856.1869999999999</v>
+        <f>jrc_potencia!W10*'SYC-SYEGC'!$G$11</f>
+        <v>878.4956776073326</v>
       </c>
       <c r="F11" s="7">
-        <f>jrc_potencia!X10</f>
-        <v>521.86599999999908</v>
+        <f>jrc_potencia!X10*'SYC-SYEGC'!$G$11</f>
+        <v>535.46366073092383</v>
       </c>
       <c r="G11" s="7">
-        <f>jrc_potencia!Y10</f>
-        <v>561.43299999999999</v>
+        <f>jrc_potencia!Y10*'SYC-SYEGC'!$G$11</f>
+        <v>576.06161243527129</v>
       </c>
       <c r="H11" s="7">
-        <f>jrc_potencia!Z10</f>
-        <v>525.84212000000025</v>
+        <f>jrc_potencia!Z10*'SYC-SYEGC'!$G$11</f>
+        <v>539.54338190591136</v>
       </c>
       <c r="I11" s="7">
-        <f>jrc_potencia!AA10</f>
-        <v>322.81999999999971</v>
+        <f>jrc_potencia!AA10*'SYC-SYEGC'!$G$11</f>
+        <v>331.23134857828825</v>
       </c>
       <c r="J11" s="7">
-        <f>jrc_potencia!AB10</f>
-        <v>448.97999999999956</v>
+        <f>jrc_potencia!AB10*'SYC-SYEGC'!$G$11</f>
+        <v>460.67855425525011</v>
       </c>
       <c r="K11" s="7">
-        <f>jrc_potencia!AC10</f>
-        <v>304.42999999999938</v>
+        <f>jrc_potencia!AC10*'SYC-SYEGC'!$G$11</f>
+        <v>312.36218154912387</v>
       </c>
       <c r="L11" s="7">
-        <f>jrc_potencia!AD10</f>
-        <v>246.07000000000062</v>
+        <f>jrc_potencia!AD10*'SYC-SYEGC'!$G$11</f>
+        <v>252.48156230921154</v>
       </c>
       <c r="M11" s="7">
-        <f>jrc_potencia!AE10</f>
-        <v>408.77600000000029</v>
+        <f>jrc_potencia!AE10*'SYC-SYEGC'!$G$11</f>
+        <v>419.4270049762672</v>
       </c>
       <c r="N11" s="7">
-        <f>jrc_potencia!AF10</f>
-        <v>304.61000000000013</v>
+        <f>jrc_potencia!AF10*'SYC-SYEGC'!$G$11</f>
+        <v>312.54687160161239</v>
       </c>
       <c r="O11" s="7">
-        <f>jrc_potencia!AG10</f>
-        <v>69.282399999999598</v>
+        <f>jrc_potencia!AG10*'SYC-SYEGC'!$G$11</f>
+        <v>71.087611624869226</v>
       </c>
       <c r="P11" s="7">
-        <f>jrc_potencia!AH10</f>
-        <v>218.48000000000002</v>
+        <f>jrc_potencia!AH10*'SYC-SYEGC'!$G$11</f>
+        <v>224.17268148622912</v>
       </c>
       <c r="Q11" s="7">
-        <f>jrc_potencia!AI10</f>
-        <v>119.96000000000049</v>
+        <f>jrc_potencia!AI10*'SYC-SYEGC'!$G$11</f>
+        <v>123.08565942460707</v>
       </c>
       <c r="R11" s="7">
-        <f>jrc_potencia!AJ10</f>
+        <f>jrc_potencia!AJ10*'SYC-SYEGC'!$G$11</f>
         <v>0</v>
       </c>
       <c r="S11" s="7">
-        <f>jrc_potencia!AK10</f>
-        <v>158.41000000000031</v>
+        <f>jrc_potencia!AK10*'SYC-SYEGC'!$G$11</f>
+        <v>162.53750674768227</v>
       </c>
       <c r="T11" s="7">
-        <f>jrc_potencia!AL10</f>
-        <v>28.099999999999909</v>
+        <f>jrc_potencia!AL10*'SYC-SYEGC'!$G$11</f>
+        <v>28.832169305030288</v>
       </c>
       <c r="U11" s="7">
-        <f>jrc_potencia!AM10</f>
-        <v>291.72000000000025</v>
+        <f>jrc_potencia!AM10*'SYC-SYEGC'!$G$11</f>
+        <v>299.32101173179609</v>
       </c>
       <c r="V11" s="7">
-        <f>jrc_potencia!AN10</f>
-        <v>390.16999999999962</v>
+        <f>jrc_potencia!AN10*'SYC-SYEGC'!$G$11</f>
+        <v>400.33620988411718</v>
       </c>
       <c r="W11" s="7">
-        <f>jrc_potencia!AO10</f>
-        <v>517.70000000000073</v>
+        <f>jrc_potencia!AO10*'SYC-SYEGC'!$G$11</f>
+        <v>531.18911207168151</v>
       </c>
       <c r="X11" s="7">
-        <f>jrc_potencia!AP10</f>
-        <v>230.59999999999945</v>
+        <f>jrc_potencia!AP10*'SYC-SYEGC'!$G$11</f>
+        <v>236.6084783537363</v>
       </c>
       <c r="Y11" s="7">
-        <f>jrc_potencia!AQ10</f>
-        <v>75.000000000000455</v>
+        <f>jrc_potencia!AQ10*'SYC-SYEGC'!$G$11</f>
+        <v>76.954188536558433</v>
       </c>
       <c r="Z11" s="7">
-        <f>jrc_potencia!AR10</f>
-        <v>57.713215000000218</v>
+        <f>jrc_potencia!AR10*'SYC-SYEGC'!$G$11</f>
+        <v>59.216981708812291</v>
       </c>
       <c r="AA11" s="7">
-        <f>jrc_potencia!AS10</f>
-        <v>234.79999999999973</v>
+        <f>jrc_potencia!AS10*'SYC-SYEGC'!$G$11</f>
+        <v>240.91791291178384</v>
       </c>
       <c r="AB11" s="7">
-        <f>jrc_potencia!AT10</f>
+        <f>jrc_potencia!AT10*'SYC-SYEGC'!$G$11</f>
         <v>0</v>
       </c>
       <c r="AC11" s="7">
-        <f>jrc_potencia!AU10</f>
-        <v>308.87595223749895</v>
+        <f>jrc_potencia!AU10*'SYC-SYEGC'!$G$11</f>
+        <v>316.9239768385782</v>
       </c>
       <c r="AD11" s="7">
-        <f>jrc_potencia!AV10</f>
-        <v>128.65000000000055</v>
+        <f>jrc_potencia!AV10*'SYC-SYEGC'!$G$11</f>
+        <v>132.0020847363763</v>
       </c>
       <c r="AE11" s="7">
-        <f>jrc_potencia!AW10</f>
+        <f>jrc_potencia!AW10*'SYC-SYEGC'!$G$11</f>
         <v>0</v>
       </c>
       <c r="AF11" s="7">
-        <f>jrc_potencia!AX10</f>
+        <f>jrc_potencia!AX10*'SYC-SYEGC'!$G$11</f>
         <v>0</v>
       </c>
       <c r="AG11" s="7">
-        <f>jrc_potencia!AY10</f>
+        <f>jrc_potencia!AY10*'SYC-SYEGC'!$G$11</f>
         <v>0</v>
       </c>
       <c r="AH11" s="7">
-        <f>jrc_potencia!AZ10</f>
+        <f>jrc_potencia!AZ10*'SYC-SYEGC'!$G$11</f>
         <v>0</v>
       </c>
       <c r="AJ11" s="1"/>
@@ -42089,136 +41903,136 @@
         <v>12</v>
       </c>
       <c r="B12" s="1">
-        <f>jrc_potencia!T45</f>
-        <v>288.05000000000064</v>
+        <f>jrc_potencia!T45*'SYC-SYEGC'!$G$12</f>
+        <v>275.93547089037338</v>
       </c>
       <c r="C12" s="1">
-        <f>jrc_potencia!U45</f>
-        <v>512.20999999999958</v>
+        <f>jrc_potencia!U45*'SYC-SYEGC'!$G$12</f>
+        <v>490.66796578634865</v>
       </c>
       <c r="D12" s="1">
-        <f>jrc_potencia!V45</f>
-        <v>423.9092499999997</v>
+        <f>jrc_potencia!V45*'SYC-SYEGC'!$G$12</f>
+        <v>406.08088357415267</v>
       </c>
       <c r="E12" s="1">
-        <f>jrc_potencia!W45</f>
-        <v>499.65900000000056</v>
+        <f>jrc_potencia!W45*'SYC-SYEGC'!$G$12</f>
+        <v>478.64482364038508</v>
       </c>
       <c r="F12" s="1">
-        <f>jrc_potencia!X45</f>
-        <v>545.80499999999938</v>
+        <f>jrc_potencia!X45*'SYC-SYEGC'!$G$12</f>
+        <v>522.85005967477775</v>
       </c>
       <c r="G12" s="1">
-        <f>jrc_potencia!Y45</f>
-        <v>458.19500000000062</v>
+        <f>jrc_potencia!Y45*'SYC-SYEGC'!$G$12</f>
+        <v>438.92467656523007</v>
       </c>
       <c r="H12" s="1">
-        <f>jrc_potencia!Z45</f>
-        <v>296.18300000000022</v>
+        <f>jrc_potencia!Z45*'SYC-SYEGC'!$G$12</f>
+        <v>283.72642101969569</v>
       </c>
       <c r="I12" s="1">
-        <f>jrc_potencia!AA45</f>
-        <v>240.4109999999996</v>
+        <f>jrc_potencia!AA45*'SYC-SYEGC'!$G$12</f>
+        <v>230.30002601015553</v>
       </c>
       <c r="J12" s="1">
-        <f>jrc_potencia!AB45</f>
-        <v>258.90794000000028</v>
+        <f>jrc_potencia!AB45*'SYC-SYEGC'!$G$12</f>
+        <v>248.01903954576102</v>
       </c>
       <c r="K12" s="1">
-        <f>jrc_potencia!AC45</f>
-        <v>168.02864</v>
+        <f>jrc_potencia!AC45*'SYC-SYEGC'!$G$12</f>
+        <v>160.96185350275621</v>
       </c>
       <c r="L12" s="1">
-        <f>jrc_potencia!AD45</f>
-        <v>91.719780000000355</v>
+        <f>jrc_potencia!AD45*'SYC-SYEGC'!$G$12</f>
+        <v>87.862317945709052</v>
       </c>
       <c r="M12" s="1">
-        <f>jrc_potencia!AE45</f>
-        <v>365.50867999999929</v>
+        <f>jrc_potencia!AE45*'SYC-SYEGC'!$G$12</f>
+        <v>350.13646842672586</v>
       </c>
       <c r="N12" s="1">
-        <f>jrc_potencia!AF45</f>
-        <v>368.69750000000005</v>
+        <f>jrc_potencia!AF45*'SYC-SYEGC'!$G$12</f>
+        <v>353.19117611040872</v>
       </c>
       <c r="O12" s="1">
-        <f>jrc_potencia!AG45</f>
-        <v>655.5404400000001</v>
+        <f>jrc_potencia!AG45*'SYC-SYEGC'!$G$12</f>
+        <v>627.97035236619399</v>
       </c>
       <c r="P12" s="1">
-        <f>jrc_potencia!AH45</f>
-        <v>95.883200000000102</v>
+        <f>jrc_potencia!AH45*'SYC-SYEGC'!$G$12</f>
+        <v>91.85063684247811</v>
       </c>
       <c r="Q12" s="1">
-        <f>jrc_potencia!AI45</f>
-        <v>68.222200000000015</v>
+        <f>jrc_potencia!AI45*'SYC-SYEGC'!$G$12</f>
+        <v>65.352976504694297</v>
       </c>
       <c r="R12" s="1">
-        <f>jrc_potencia!AJ45</f>
-        <v>289.21559999999999</v>
+        <f>jrc_potencia!AJ45*'SYC-SYEGC'!$G$12</f>
+        <v>277.05204920965696</v>
       </c>
       <c r="S12" s="1">
-        <f>jrc_potencia!AK45</f>
-        <v>89.452200000000119</v>
+        <f>jrc_potencia!AK45*'SYC-SYEGC'!$G$12</f>
+        <v>85.690105638534405</v>
       </c>
       <c r="T12" s="1">
-        <f>jrc_potencia!AL45</f>
-        <v>95.556999999999988</v>
+        <f>jrc_potencia!AL45*'SYC-SYEGC'!$G$12</f>
+        <v>91.538155847496427</v>
       </c>
       <c r="U12" s="1">
-        <f>jrc_potencia!AM45</f>
-        <v>249.19999999999959</v>
+        <f>jrc_potencia!AM45*'SYC-SYEGC'!$G$12</f>
+        <v>238.71938672411312</v>
       </c>
       <c r="V12" s="1">
-        <f>jrc_potencia!AN45</f>
-        <v>3.7000000000000028</v>
+        <f>jrc_potencia!AN45*'SYC-SYEGC'!$G$12</f>
+        <v>3.5443889682151712</v>
       </c>
       <c r="W12" s="1">
-        <f>jrc_potencia!AO45</f>
-        <v>9.4500000000000277</v>
+        <f>jrc_potencia!AO45*'SYC-SYEGC'!$G$12</f>
+        <v>9.0525610134144436</v>
       </c>
       <c r="X12" s="1">
-        <f>jrc_potencia!AP45</f>
-        <v>514.78</v>
+        <f>jrc_potencia!AP45*'SYC-SYEGC'!$G$12</f>
+        <v>493.12987920481197</v>
       </c>
       <c r="Y12" s="1">
-        <f>jrc_potencia!AQ45</f>
-        <v>136.79999999999995</v>
+        <f>jrc_potencia!AQ45*'SYC-SYEGC'!$G$12</f>
+        <v>131.04659752752295</v>
       </c>
       <c r="Z12" s="1">
-        <f>jrc_potencia!AR45</f>
-        <v>154.65000000000009</v>
+        <f>jrc_potencia!AR45*'SYC-SYEGC'!$G$12</f>
+        <v>148.14587944175031</v>
       </c>
       <c r="AA12" s="1">
-        <f>jrc_potencia!AS45</f>
+        <f>jrc_potencia!AS45*'SYC-SYEGC'!$G$12</f>
         <v>0</v>
       </c>
       <c r="AB12" s="1">
-        <f>jrc_potencia!AT45</f>
-        <v>10.9</v>
+        <f>jrc_potencia!AT45*'SYC-SYEGC'!$G$12</f>
+        <v>10.44157831176901</v>
       </c>
       <c r="AC12" s="1">
-        <f>jrc_potencia!AU45</f>
-        <v>774.25</v>
+        <f>jrc_potencia!AU45*'SYC-SYEGC'!$G$12</f>
+        <v>741.68734017313352</v>
       </c>
       <c r="AD12" s="1">
-        <f>jrc_potencia!AV45</f>
-        <v>146.25</v>
+        <f>jrc_potencia!AV45*'SYC-SYEGC'!$G$12</f>
+        <v>140.0991585409374</v>
       </c>
       <c r="AE12" s="1">
-        <f>jrc_potencia!AW45</f>
-        <v>3.8000000000000003</v>
+        <f>jrc_potencia!AW45*'SYC-SYEGC'!$G$12</f>
+        <v>3.6401832646534165</v>
       </c>
       <c r="AF12" s="1">
-        <f>jrc_potencia!AX45</f>
+        <f>jrc_potencia!AX45*'SYC-SYEGC'!$G$12</f>
         <v>0</v>
       </c>
       <c r="AG12" s="1">
-        <f>jrc_potencia!AY45</f>
+        <f>jrc_potencia!AY45*'SYC-SYEGC'!$G$12</f>
         <v>0</v>
       </c>
       <c r="AH12" s="1">
-        <f>jrc_potencia!AZ45</f>
-        <v>276.55</v>
+        <f>jrc_potencia!AZ45*'SYC-SYEGC'!$G$12</f>
+        <v>264.91912679997426</v>
       </c>
       <c r="AJ12" s="1"/>
     </row>
@@ -42227,136 +42041,136 @@
         <v>18</v>
       </c>
       <c r="B13" s="1">
-        <f>jrc_potencia!T6</f>
-        <v>1054.2000000000044</v>
+        <f>jrc_potencia!T6*'SYC-SYEGC'!$G$13</f>
+        <v>947.68019473641971</v>
       </c>
       <c r="C13" s="1">
-        <f>jrc_potencia!U6</f>
-        <v>1921.7999999999956</v>
+        <f>jrc_potencia!U6*'SYC-SYEGC'!$G$13</f>
+        <v>1727.6150618900017</v>
       </c>
       <c r="D13" s="1">
-        <f>jrc_potencia!V6</f>
-        <v>4394.9200000000055</v>
+        <f>jrc_potencia!V6*'SYC-SYEGC'!$G$13</f>
+        <v>3950.8429533778917</v>
       </c>
       <c r="E13" s="1">
-        <f>jrc_potencia!W6</f>
-        <v>2642.5</v>
+        <f>jrc_potencia!W6*'SYC-SYEGC'!$G$13</f>
+        <v>2375.4931840172439</v>
       </c>
       <c r="F13" s="1">
-        <f>jrc_potencia!X6</f>
-        <v>1550</v>
+        <f>jrc_potencia!X6*'SYC-SYEGC'!$G$13</f>
+        <v>1393.3829461595944</v>
       </c>
       <c r="G13" s="1">
-        <f>jrc_potencia!Y6</f>
-        <v>1641</v>
+        <f>jrc_potencia!Y6*'SYC-SYEGC'!$G$13</f>
+        <v>1475.1880094502544</v>
       </c>
       <c r="H13" s="1">
-        <f>jrc_potencia!Z6</f>
-        <v>681.40000000000146</v>
+        <f>jrc_potencia!Z6*'SYC-SYEGC'!$G$13</f>
+        <v>612.54912226654812</v>
       </c>
       <c r="I13" s="1">
-        <f>jrc_potencia!AA6</f>
-        <v>2619.7999999999956</v>
+        <f>jrc_potencia!AA6*'SYC-SYEGC'!$G$13</f>
+        <v>2355.0868660315482</v>
       </c>
       <c r="J13" s="1">
-        <f>jrc_potencia!AB6</f>
-        <v>1190</v>
+        <f>jrc_potencia!AB6*'SYC-SYEGC'!$G$13</f>
+        <v>1069.7585199547855</v>
       </c>
       <c r="K13" s="1">
-        <f>jrc_potencia!AC6</f>
-        <v>1845.75</v>
+        <f>jrc_potencia!AC6*'SYC-SYEGC'!$G$13</f>
+        <v>1659.2494018542395</v>
       </c>
       <c r="L13" s="1">
-        <f>jrc_potencia!AD6</f>
-        <v>1764</v>
+        <f>jrc_potencia!AD6*'SYC-SYEGC'!$G$13</f>
+        <v>1585.7596884035643</v>
       </c>
       <c r="M13" s="1">
-        <f>jrc_potencia!AE6</f>
-        <v>744</v>
+        <f>jrc_potencia!AE6*'SYC-SYEGC'!$G$13</f>
+        <v>668.82381415660529</v>
       </c>
       <c r="N13" s="1">
-        <f>jrc_potencia!AF6</f>
-        <v>1916</v>
+        <f>jrc_potencia!AF6*'SYC-SYEGC'!$G$13</f>
+        <v>1722.4011128011502</v>
       </c>
       <c r="O13" s="1">
-        <f>jrc_potencia!AG6</f>
-        <v>3113.1000000000022</v>
+        <f>jrc_potencia!AG6*'SYC-SYEGC'!$G$13</f>
+        <v>2798.5422256060879</v>
       </c>
       <c r="P13" s="1">
-        <f>jrc_potencia!AH6</f>
-        <v>780.79999999999927</v>
+        <f>jrc_potencia!AH6*'SYC-SYEGC'!$G$13</f>
+        <v>701.90542216865185</v>
       </c>
       <c r="Q13" s="1">
-        <f>jrc_potencia!AI6</f>
-        <v>724</v>
+        <f>jrc_potencia!AI6*'SYC-SYEGC'!$G$13</f>
+        <v>650.84467936744932</v>
       </c>
       <c r="R13" s="1">
-        <f>jrc_potencia!AJ6</f>
-        <v>1685.0200000000004</v>
+        <f>jrc_potencia!AJ6*'SYC-SYEGC'!$G$13</f>
+        <v>1514.7600851211873</v>
       </c>
       <c r="S13" s="1">
-        <f>jrc_potencia!AK6</f>
-        <v>3471.7800000000025</v>
+        <f>jrc_potencia!AK6*'SYC-SYEGC'!$G$13</f>
+        <v>3120.9800289148129</v>
       </c>
       <c r="T13" s="1">
-        <f>jrc_potencia!AL6</f>
-        <v>1243.3999999999978</v>
+        <f>jrc_potencia!AL6*'SYC-SYEGC'!$G$13</f>
+        <v>1117.7628098418302</v>
       </c>
       <c r="U13" s="1">
-        <f>jrc_potencia!AM6</f>
-        <v>1845.5</v>
+        <f>jrc_potencia!AM6*'SYC-SYEGC'!$G$13</f>
+        <v>1659.0246626693752</v>
       </c>
       <c r="V13" s="1">
-        <f>jrc_potencia!AN6</f>
-        <v>1518.9000000000015</v>
+        <f>jrc_potencia!AN6*'SYC-SYEGC'!$G$13</f>
+        <v>1365.4253915624581</v>
       </c>
       <c r="W13" s="1">
-        <f>jrc_potencia!AO6</f>
-        <v>369.02500000000146</v>
+        <f>jrc_potencia!AO6*'SYC-SYEGC'!$G$13</f>
+        <v>331.737510778417</v>
       </c>
       <c r="X13" s="1">
-        <f>jrc_potencia!AP6</f>
-        <v>205.39999999999782</v>
+        <f>jrc_potencia!AP6*'SYC-SYEGC'!$G$13</f>
+        <v>184.64571428463074</v>
       </c>
       <c r="Y13" s="1">
-        <f>jrc_potencia!AQ6</f>
-        <v>1306.2000000000007</v>
+        <f>jrc_potencia!AQ6*'SYC-SYEGC'!$G$13</f>
+        <v>1174.2172930797828</v>
       </c>
       <c r="Z13" s="1">
-        <f>jrc_potencia!AR6</f>
-        <v>835</v>
+        <f>jrc_potencia!AR6*'SYC-SYEGC'!$G$13</f>
+        <v>750.62887744726538</v>
       </c>
       <c r="AA13" s="1">
-        <f>jrc_potencia!AS6</f>
-        <v>1897.7000000000007</v>
+        <f>jrc_potencia!AS6*'SYC-SYEGC'!$G$13</f>
+        <v>1705.9502044690732</v>
       </c>
       <c r="AB13" s="1">
-        <f>jrc_potencia!AT6</f>
-        <v>2731.6000000000004</v>
+        <f>jrc_potencia!AT6*'SYC-SYEGC'!$G$13</f>
+        <v>2455.5902295029346</v>
       </c>
       <c r="AC13" s="1">
-        <f>jrc_potencia!AU6</f>
-        <v>824.79999999999927</v>
+        <f>jrc_potencia!AU6*'SYC-SYEGC'!$G$13</f>
+        <v>741.45951870479519</v>
       </c>
       <c r="AD13" s="1">
-        <f>jrc_potencia!AV6</f>
-        <v>293.5</v>
+        <f>jrc_potencia!AV6*'SYC-SYEGC'!$G$13</f>
+        <v>263.84380303086516</v>
       </c>
       <c r="AE13" s="1">
-        <f>jrc_potencia!AW6</f>
-        <v>1351.4400000000005</v>
+        <f>jrc_potencia!AW6*'SYC-SYEGC'!$G$13</f>
+        <v>1214.8860959728536</v>
       </c>
       <c r="AF13" s="1">
-        <f>jrc_potencia!AX6</f>
-        <v>648.86000000000058</v>
+        <f>jrc_potencia!AX6*'SYC-SYEGC'!$G$13</f>
+        <v>583.29706996459049</v>
       </c>
       <c r="AG13" s="1">
-        <f>jrc_potencia!AY6</f>
-        <v>415.40999999999985</v>
+        <f>jrc_potencia!AY6*'SYC-SYEGC'!$G$13</f>
+        <v>373.43561913816575</v>
       </c>
       <c r="AH13" s="1">
-        <f>jrc_potencia!AZ6</f>
-        <v>24</v>
+        <f>jrc_potencia!AZ6*'SYC-SYEGC'!$G$13</f>
+        <v>21.57496174698727</v>
       </c>
       <c r="AJ13" s="1"/>
     </row>
@@ -42365,136 +42179,136 @@
         <v>19</v>
       </c>
       <c r="B14">
-        <f>jrc_potencia!T16</f>
+        <f>jrc_potencia!T16*'SYC-SYEGC'!$G$14</f>
         <v>0</v>
       </c>
       <c r="C14">
-        <f>jrc_potencia!U16</f>
-        <v>12.999999999996362</v>
+        <f>jrc_potencia!U16*'SYC-SYEGC'!$G$14</f>
+        <v>11.973823420773055</v>
       </c>
       <c r="D14">
-        <f>jrc_potencia!V16</f>
-        <v>5</v>
+        <f>jrc_potencia!V16*'SYC-SYEGC'!$G$14</f>
+        <v>4.6053167002986175</v>
       </c>
       <c r="E14">
-        <f>jrc_potencia!W16</f>
+        <f>jrc_potencia!W16*'SYC-SYEGC'!$G$14</f>
         <v>0</v>
       </c>
       <c r="F14">
-        <f>jrc_potencia!X16</f>
+        <f>jrc_potencia!X16*'SYC-SYEGC'!$G$14</f>
         <v>0</v>
       </c>
       <c r="G14">
-        <f>jrc_potencia!Y16</f>
-        <v>2.749999999992724</v>
+        <f>jrc_potencia!Y16*'SYC-SYEGC'!$G$14</f>
+        <v>2.5329241851575381</v>
       </c>
       <c r="H14">
-        <f>jrc_potencia!Z16</f>
+        <f>jrc_potencia!Z16*'SYC-SYEGC'!$G$14</f>
         <v>0</v>
       </c>
       <c r="I14">
-        <f>jrc_potencia!AA16</f>
-        <v>14.5</v>
+        <f>jrc_potencia!AA16*'SYC-SYEGC'!$G$14</f>
+        <v>13.355418430865992</v>
       </c>
       <c r="J14">
-        <f>jrc_potencia!AB16</f>
-        <v>40</v>
+        <f>jrc_potencia!AB16*'SYC-SYEGC'!$G$14</f>
+        <v>36.84253360238894</v>
       </c>
       <c r="K14">
-        <f>jrc_potencia!AC16</f>
-        <v>6.2999999999956344</v>
+        <f>jrc_potencia!AC16*'SYC-SYEGC'!$G$14</f>
+        <v>5.8026990423722378</v>
       </c>
       <c r="L14">
-        <f>jrc_potencia!AD16</f>
-        <v>292.30000000000291</v>
+        <f>jrc_potencia!AD16*'SYC-SYEGC'!$G$14</f>
+        <v>269.22681429945987</v>
       </c>
       <c r="M14">
-        <f>jrc_potencia!AE16</f>
-        <v>220</v>
+        <f>jrc_potencia!AE16*'SYC-SYEGC'!$G$14</f>
+        <v>202.63393481313918</v>
       </c>
       <c r="N14">
-        <f>jrc_potencia!AF16</f>
-        <v>93.000000000021828</v>
+        <f>jrc_potencia!AF16*'SYC-SYEGC'!$G$14</f>
+        <v>85.658890625574401</v>
       </c>
       <c r="O14">
-        <f>jrc_potencia!AG16</f>
-        <v>200.4999999999709</v>
+        <f>jrc_potencia!AG16*'SYC-SYEGC'!$G$14</f>
+        <v>184.67319968194778</v>
       </c>
       <c r="P14">
-        <f>jrc_potencia!AH16</f>
-        <v>210.39999999999418</v>
+        <f>jrc_potencia!AH16*'SYC-SYEGC'!$G$14</f>
+        <v>193.79172674856048</v>
       </c>
       <c r="Q14">
-        <f>jrc_potencia!AI16</f>
-        <v>347.5000000000291</v>
+        <f>jrc_potencia!AI16*'SYC-SYEGC'!$G$14</f>
+        <v>320.06951067078074</v>
       </c>
       <c r="R14">
-        <f>jrc_potencia!AJ16</f>
-        <v>419.50000000001455</v>
+        <f>jrc_potencia!AJ16*'SYC-SYEGC'!$G$14</f>
+        <v>386.38607115506744</v>
       </c>
       <c r="S14">
-        <f>jrc_potencia!AK16</f>
-        <v>1133.8000000000029</v>
+        <f>jrc_potencia!AK16*'SYC-SYEGC'!$G$14</f>
+        <v>1044.3016149597172</v>
       </c>
       <c r="T14">
-        <f>jrc_potencia!AL16</f>
-        <v>501.59999999999127</v>
+        <f>jrc_potencia!AL16*'SYC-SYEGC'!$G$14</f>
+        <v>462.00537137394929</v>
       </c>
       <c r="U14">
-        <f>jrc_potencia!AM16</f>
-        <v>1622.8999999999942</v>
+        <f>jrc_potencia!AM16*'SYC-SYEGC'!$G$14</f>
+        <v>1494.7936945829201</v>
       </c>
       <c r="V14">
-        <f>jrc_potencia!AN16</f>
-        <v>1809.8000000000029</v>
+        <f>jrc_potencia!AN16*'SYC-SYEGC'!$G$14</f>
+        <v>1666.9404328400904</v>
       </c>
       <c r="W14">
-        <f>jrc_potencia!AO16</f>
-        <v>1030.5000000000146</v>
+        <f>jrc_potencia!AO16*'SYC-SYEGC'!$G$14</f>
+        <v>949.15577193155855</v>
       </c>
       <c r="X14">
-        <f>jrc_potencia!AP16</f>
-        <v>3010.3999999999796</v>
+        <f>jrc_potencia!AP16*'SYC-SYEGC'!$G$14</f>
+        <v>2772.7690789157732</v>
       </c>
       <c r="Y14">
-        <f>jrc_potencia!AQ16</f>
-        <v>1660.7999999999884</v>
+        <f>jrc_potencia!AQ16*'SYC-SYEGC'!$G$14</f>
+        <v>1529.7019951711782</v>
       </c>
       <c r="Z14">
-        <f>jrc_potencia!AR16</f>
-        <v>3222.8000000000175</v>
+        <f>jrc_potencia!AR16*'SYC-SYEGC'!$G$14</f>
+        <v>2968.4029323444934</v>
       </c>
       <c r="AA14">
-        <f>jrc_potencia!AS16</f>
-        <v>3769.1999999999825</v>
+        <f>jrc_potencia!AS16*'SYC-SYEGC'!$G$14</f>
+        <v>3471.6719413530941</v>
       </c>
       <c r="AB14">
-        <f>jrc_potencia!AT16</f>
-        <v>3858.8000000000029</v>
+        <f>jrc_potencia!AT16*'SYC-SYEGC'!$G$14</f>
+        <v>3554.1992166224641</v>
       </c>
       <c r="AC14">
-        <f>jrc_potencia!AU16</f>
-        <v>6498.3400000000402</v>
+        <f>jrc_potencia!AU16*'SYC-SYEGC'!$G$14</f>
+        <v>5985.3827452437408</v>
       </c>
       <c r="AD14">
-        <f>jrc_potencia!AV16</f>
-        <v>1504.5733333333628</v>
+        <f>jrc_potencia!AV16*'SYC-SYEGC'!$G$14</f>
+        <v>1385.8073397648191</v>
       </c>
       <c r="AE14">
-        <f>jrc_potencia!AW16</f>
-        <v>698.38333333330229</v>
+        <f>jrc_potencia!AW16*'SYC-SYEGC'!$G$14</f>
+        <v>643.25528564201466</v>
       </c>
       <c r="AF14">
-        <f>jrc_potencia!AX16</f>
-        <v>3702.3150000000023</v>
+        <f>jrc_potencia!AX16*'SYC-SYEGC'!$G$14</f>
+        <v>3410.0666198532176</v>
       </c>
       <c r="AG14">
-        <f>jrc_potencia!AY16</f>
-        <v>4033.6999999999825</v>
+        <f>jrc_potencia!AY16*'SYC-SYEGC'!$G$14</f>
+        <v>3715.2931947988909</v>
       </c>
       <c r="AH14">
-        <f>jrc_potencia!AZ16</f>
-        <v>2332.8250000000116</v>
+        <f>jrc_potencia!AZ16*'SYC-SYEGC'!$G$14</f>
+        <v>2148.6795862748354</v>
       </c>
       <c r="AJ14" s="1"/>
     </row>
@@ -42505,100 +42319,100 @@
       <c r="B15">
         <v>0</v>
       </c>
-      <c r="C15" s="1">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0</v>
-      </c>
-      <c r="F15" s="1">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1">
-        <v>0</v>
-      </c>
-      <c r="J15" s="1">
-        <v>0</v>
-      </c>
-      <c r="K15" s="1">
-        <v>0</v>
-      </c>
-      <c r="L15" s="1">
-        <v>0</v>
-      </c>
-      <c r="M15" s="1">
-        <v>0</v>
-      </c>
-      <c r="N15" s="1">
-        <v>0</v>
-      </c>
-      <c r="O15" s="1">
-        <v>0</v>
-      </c>
-      <c r="P15" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="1">
-        <v>0</v>
-      </c>
-      <c r="R15" s="1">
-        <v>0</v>
-      </c>
-      <c r="S15" s="1">
-        <v>0</v>
-      </c>
-      <c r="T15" s="1">
-        <v>0</v>
-      </c>
-      <c r="U15" s="1">
-        <v>0</v>
-      </c>
-      <c r="V15" s="1">
-        <v>0</v>
-      </c>
-      <c r="W15" s="1">
-        <v>0</v>
-      </c>
-      <c r="X15" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA15" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB15" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC15" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD15" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE15" s="1">
-        <v>0</v>
-      </c>
-      <c r="AF15" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG15" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH15" s="1">
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+      <c r="AE15">
+        <v>0</v>
+      </c>
+      <c r="AF15">
+        <v>0</v>
+      </c>
+      <c r="AG15">
+        <v>0</v>
+      </c>
+      <c r="AH15">
         <v>0</v>
       </c>
     </row>
@@ -42607,103 +42421,135 @@
         <v>31</v>
       </c>
       <c r="B16">
-        <f>jrc_potencia!T11</f>
-        <v>1997</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1">
-        <v>0</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1">
-        <v>0</v>
-      </c>
-      <c r="H16" s="1">
-        <v>0</v>
-      </c>
-      <c r="I16" s="1">
-        <v>0</v>
-      </c>
-      <c r="J16" s="1">
-        <v>0</v>
-      </c>
-      <c r="K16" s="1">
-        <v>0</v>
-      </c>
-      <c r="L16" s="1">
-        <v>0</v>
-      </c>
-      <c r="M16" s="1">
-        <v>0</v>
-      </c>
-      <c r="N16" s="1">
-        <v>0</v>
-      </c>
-      <c r="O16" s="1">
-        <v>0</v>
-      </c>
-      <c r="P16" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="1">
-        <v>0</v>
-      </c>
-      <c r="R16" s="1">
-        <v>0</v>
-      </c>
-      <c r="S16" s="1">
-        <v>0</v>
-      </c>
-      <c r="T16" s="1">
-        <v>0</v>
-      </c>
-      <c r="U16" s="1">
-        <v>0</v>
-      </c>
-      <c r="V16" s="1">
-        <v>0</v>
-      </c>
-      <c r="W16" s="1">
-        <v>0</v>
-      </c>
-      <c r="X16" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z16" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB16" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC16" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD16" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE16" s="1">
-        <v>0</v>
-      </c>
-      <c r="AF16" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG16" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH16" s="1">
+        <f>jrc_potencia!T11*'SYC-SYEGC'!$G$16</f>
+        <v>1761.6449281161665</v>
+      </c>
+      <c r="C16">
+        <f>jrc_potencia!U11*'SYC-SYEGC'!$G$16</f>
+        <v>1540.7644706544709</v>
+      </c>
+      <c r="D16">
+        <f>jrc_potencia!V11*'SYC-SYEGC'!$G$16</f>
+        <v>2440.4207450356776</v>
+      </c>
+      <c r="E16">
+        <f>jrc_potencia!W11*'SYC-SYEGC'!$G$16</f>
+        <v>1058.7512482348643</v>
+      </c>
+      <c r="F16">
+        <f>jrc_potencia!X11*'SYC-SYEGC'!$G$16</f>
+        <v>1964.5825423941465</v>
+      </c>
+      <c r="G16">
+        <f>jrc_potencia!Y11*'SYC-SYEGC'!$G$16</f>
+        <v>2830.1174217730827</v>
+      </c>
+      <c r="H16">
+        <f>jrc_potencia!Z11*'SYC-SYEGC'!$G$16</f>
+        <v>1522.671662704714</v>
+      </c>
+      <c r="I16">
+        <f>jrc_potencia!AA11*'SYC-SYEGC'!$G$16</f>
+        <v>321.8949595741563</v>
+      </c>
+      <c r="J16">
+        <f>jrc_potencia!AB11*'SYC-SYEGC'!$G$16</f>
+        <v>105.76926734157622</v>
+      </c>
+      <c r="K16">
+        <f>jrc_potencia!AC11*'SYC-SYEGC'!$G$16</f>
+        <v>59.6683339698438</v>
+      </c>
+      <c r="L16">
+        <f>jrc_potencia!AD11*'SYC-SYEGC'!$G$16</f>
+        <v>371.84645885035872</v>
+      </c>
+      <c r="M16">
+        <f>jrc_potencia!AE11*'SYC-SYEGC'!$G$16</f>
+        <v>1019.5398726440958</v>
+      </c>
+      <c r="N16">
+        <f>jrc_potencia!AF11*'SYC-SYEGC'!$G$16</f>
+        <v>364.06152320157395</v>
+      </c>
+      <c r="O16">
+        <f>jrc_potencia!AG11*'SYC-SYEGC'!$G$16</f>
+        <v>133.55685634290785</v>
+      </c>
+      <c r="P16">
+        <f>jrc_potencia!AH11*'SYC-SYEGC'!$G$16</f>
+        <v>86.891349734322674</v>
+      </c>
+      <c r="Q16">
+        <f>jrc_potencia!AI11*'SYC-SYEGC'!$G$16</f>
+        <v>970.16617878998352</v>
+      </c>
+      <c r="R16">
+        <f>jrc_potencia!AJ11*'SYC-SYEGC'!$G$16</f>
+        <v>116.47851592812145</v>
+      </c>
+      <c r="S16">
+        <f>jrc_potencia!AK11*'SYC-SYEGC'!$G$16</f>
+        <v>141.05509464485488</v>
+      </c>
+      <c r="T16">
+        <f>jrc_potencia!AL11*'SYC-SYEGC'!$G$16</f>
+        <v>936.30942749248834</v>
+      </c>
+      <c r="U16">
+        <f>jrc_potencia!AM11*'SYC-SYEGC'!$G$16</f>
+        <v>660.55068711736897</v>
+      </c>
+      <c r="V16">
+        <f>jrc_potencia!AN11*'SYC-SYEGC'!$G$16</f>
+        <v>217.23278506421971</v>
+      </c>
+      <c r="W16">
+        <f>jrc_potencia!AO11*'SYC-SYEGC'!$G$16</f>
+        <v>324.62961119015966</v>
+      </c>
+      <c r="X16">
+        <f>jrc_potencia!AP11*'SYC-SYEGC'!$G$16</f>
+        <v>477.15259970858017</v>
+      </c>
+      <c r="Y16">
+        <f>jrc_potencia!AQ11*'SYC-SYEGC'!$G$16</f>
+        <v>670.43071876228669</v>
+      </c>
+      <c r="Z16">
+        <f>jrc_potencia!AR11*'SYC-SYEGC'!$G$16</f>
+        <v>24.700079112294798</v>
+      </c>
+      <c r="AA16">
+        <f>jrc_potencia!AS11*'SYC-SYEGC'!$G$16</f>
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <f>jrc_potencia!AT11*'SYC-SYEGC'!$G$16</f>
+        <v>2.9110807525204403</v>
+      </c>
+      <c r="AC16">
+        <f>jrc_potencia!AU11*'SYC-SYEGC'!$G$16</f>
+        <v>101.44675349692496</v>
+      </c>
+      <c r="AD16">
+        <f>jrc_potencia!AV11*'SYC-SYEGC'!$G$16</f>
+        <v>11.360272100290432</v>
+      </c>
+      <c r="AE16">
+        <f>jrc_potencia!AW11*'SYC-SYEGC'!$G$16</f>
+        <v>0</v>
+      </c>
+      <c r="AF16">
+        <f>jrc_potencia!AX11*'SYC-SYEGC'!$G$16</f>
+        <v>81.157402797539959</v>
+      </c>
+      <c r="AG16">
+        <f>jrc_potencia!AY11*'SYC-SYEGC'!$G$16</f>
+        <v>0</v>
+      </c>
+      <c r="AH16">
+        <f>jrc_potencia!AZ11*'SYC-SYEGC'!$G$16</f>
         <v>0</v>
       </c>
     </row>
@@ -42714,100 +42560,100 @@
       <c r="B17">
         <v>0</v>
       </c>
-      <c r="C17" s="1">
-        <v>0</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0</v>
-      </c>
-      <c r="F17" s="1">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1">
-        <v>0</v>
-      </c>
-      <c r="H17" s="1">
-        <v>0</v>
-      </c>
-      <c r="I17" s="1">
-        <v>0</v>
-      </c>
-      <c r="J17" s="1">
-        <v>0</v>
-      </c>
-      <c r="K17" s="1">
-        <v>0</v>
-      </c>
-      <c r="L17" s="1">
-        <v>0</v>
-      </c>
-      <c r="M17" s="1">
-        <v>0</v>
-      </c>
-      <c r="N17" s="1">
-        <v>0</v>
-      </c>
-      <c r="O17" s="1">
-        <v>0</v>
-      </c>
-      <c r="P17" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="1">
-        <v>0</v>
-      </c>
-      <c r="R17" s="1">
-        <v>0</v>
-      </c>
-      <c r="S17" s="1">
-        <v>0</v>
-      </c>
-      <c r="T17" s="1">
-        <v>0</v>
-      </c>
-      <c r="U17" s="1">
-        <v>0</v>
-      </c>
-      <c r="V17" s="1">
-        <v>0</v>
-      </c>
-      <c r="W17" s="1">
-        <v>0</v>
-      </c>
-      <c r="X17" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC17" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD17" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE17" s="1">
-        <v>0</v>
-      </c>
-      <c r="AF17" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG17" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH17" s="1">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
+        <v>0</v>
+      </c>
+      <c r="AA17">
+        <v>0</v>
+      </c>
+      <c r="AB17">
+        <v>0</v>
+      </c>
+      <c r="AC17">
+        <v>0</v>
+      </c>
+      <c r="AD17">
+        <v>0</v>
+      </c>
+      <c r="AE17">
+        <v>0</v>
+      </c>
+      <c r="AF17">
+        <v>0</v>
+      </c>
+      <c r="AG17">
+        <v>0</v>
+      </c>
+      <c r="AH17">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates to capacity retirements reflecting 2020 retirements and capacity factors for hydro and nuclear
</commit_message>
<xml_diff>
--- a/InputData/elec/BCRbQ/BAU Cap Retirements before Quantization.xlsx
+++ b/InputData/elec/BCRbQ/BAU Cap Retirements before Quantization.xlsx
@@ -1,34 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\European Union\Models\eps-eu\InputData\elec\BCRbQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320A9998-F196-4AA7-8996-25F2D706BF4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DC6B6C-6A13-410E-B2C1-343A9A4E16FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="14" r:id="rId1"/>
-    <sheet name="Gross Capacities" sheetId="21" r:id="rId2"/>
-    <sheet name="jrc_potencia" sheetId="19" r:id="rId3"/>
-    <sheet name="SYC-SYEGC" sheetId="20" r:id="rId4"/>
-    <sheet name="BCRbQ" sheetId="2" r:id="rId5"/>
+    <sheet name="Nuclear" sheetId="22" r:id="rId2"/>
+    <sheet name="Gross Capacities" sheetId="21" r:id="rId3"/>
+    <sheet name="jrc_potencia" sheetId="19" r:id="rId4"/>
+    <sheet name="SYC-SYEGC" sheetId="20" r:id="rId5"/>
+    <sheet name="BCRbQ" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="Countries">#REF!</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Gross Capacities'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">'Gross Capacities'!$1:$1</definedName>
     <definedName name="qry_ForHeadlineStats">#REF!</definedName>
     <definedName name="qry_plants_readout_full">#REF!</definedName>
     <definedName name="qry_plants_readout_headline">#REF!</definedName>
     <definedName name="qry_units_readout_full">#REF!</definedName>
     <definedName name="qry_units_readout_headline">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="112">
   <si>
     <t>nuclear</t>
   </si>
@@ -338,6 +339,51 @@
   </si>
   <si>
     <t>EU28: Gross capacities decommissioned (MW)</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>MW Retired</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Fessenheim 1</t>
+  </si>
+  <si>
+    <t>Fessenheim 2</t>
+  </si>
+  <si>
+    <t>Plant</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Fessenheim_Nuclear_Power_Plant</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Ringhals 2</t>
+  </si>
+  <si>
+    <t>End 2019 retirement, so effectively online all of 2019 but not at all in 2020</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Philippsburg</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Philippsburg_Nuclear_Power_Plant</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Ringhals_Nuclear_Power_Plant</t>
   </si>
 </sst>
 </file>
@@ -1289,6 +1335,100 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D60EFB-41FA-4F19-8E28-F971995C73AF}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2">
+        <v>880</v>
+      </c>
+      <c r="E2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3">
+        <v>880</v>
+      </c>
+      <c r="E3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4">
+        <v>1120</v>
+      </c>
+      <c r="D4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5">
+        <v>1402</v>
+      </c>
+      <c r="D5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -1296,11 +1436,11 @@
   <dimension ref="A1:AZ209"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B95" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
       <selection pane="topRight" activeCell="B2" sqref="B2"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="T1" sqref="B1:T1048576"/>
+      <selection pane="bottomRight" activeCell="U57" sqref="U57:W57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33922,11 +34062,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AZ46"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="U46" sqref="U46"/>
     </sheetView>
   </sheetViews>
@@ -40392,7 +40532,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
@@ -40787,7 +40927,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
@@ -40795,7 +40935,7 @@
   <dimension ref="A1:AJ23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41198,8 +41338,8 @@
         <v>2739.9999999999854</v>
       </c>
       <c r="D4" s="1">
-        <f>jrc_potencia!V3</f>
-        <v>914.00000000001455</v>
+        <f>SUM(Nuclear!C2:C5)</f>
+        <v>4282</v>
       </c>
       <c r="E4" s="1">
         <f>jrc_potencia!W3</f>
@@ -43051,6 +43191,10 @@
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" s="28"/>
       <c r="B20" s="1"/>
+      <c r="C20">
+        <f>119214</f>
+        <v>119214</v>
+      </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="30"/>

</xml_diff>